<commit_message>
Update atcc analysis in supplemental files
Also:
 - Make column labels and other labelling more uniform
   in supplemental Files
</commit_message>
<xml_diff>
--- a/inst/manuscript/supplement_files/sfile_S4.xlsx
+++ b/inst/manuscript/supplement_files/sfile_S4.xlsx
@@ -416,11 +416,11 @@
         </is>
       </c>
       <c r="F2">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>orf19.6066 UBP6 TUB2 orf19.3341 RPS4A;RPS42 HGT1 orf19.3690.2 GSC1 FRS2 RPS16A RPL6 ECM33 CDC12 RPN3 orf19.1054 CDC3 ATP1 PIL1 SEC21 YBN5 orf19.2478.1 orf19.2489 RPS14B orf19.6264.3 RPS23A RAC1 ADE5,7 orf19.1229 DPM1 orf19.5085 DAK2 IDH1 ERO1 RPS17B RPL2 orf19.1152 SAM2 GAD1 orf19.5281 RPL27A PEP1 CHS3 RPN1 RPL14 SEC18 ACT1 orf19.5006.1 GND1 RPL4B GDI1 HGT7 KAR2 orf19.1993 PLB4.5 MSB2 ARO3 orf19.1564 IDH2 ALD5 LHS1 RPL21A RPS9B RPL39 ERG10 RHO3 CYT1 orf19.6883 orf19.6882.1 COX9 VAS1 RPL11 GDH2 RPS10 PHM7 orf19.2175 orf19.2168.3 RPT6 ASN1 PMA1 KGD1 ARF3 orf19.1672 RNA1 RIP1 orf19.5917.3 RPS15 RPL35 RPL19A RPL18 RPS19A FAS2 YCK2 CAM1 UBA1 LYS9 CYP5 orf19.6741 FUM12 VMA6 SUB2 PRO3 ATP2 CAR2 RPS6A RPL20B IDI1 orf19.2720 NCP1 RPN6 PYC2 orf19.1409.1 orf19.3799 RPL30 LYS1 TRP5 GDH3 CCT6 GUT2 RPT5 orf19.5682 THS1 VPS1 orf19.4149.1 orf19.4246 CAM1-1 RPS25B RPL43A MES1 orf19.3983 ADH1 orf19.4016 HET1 FET34 RPS13 ILV5 RPL32 RPL25 CHC1 RPL23A SAC6 orf19.5627 GUS1 GLN4 GPH1 RPS18 RPP0 orf19.6507 PDI1 SHM1 SUI3 YRB1 ACC1 CRM1 ATP3 CDC60 FRS1 VMA4 ADH5 ECM4 IDP2 RPL28 ARC1 IFR2 CIT1 PRE6 RPS3 VMA13 GLN1 PST3 YCP4 LSC2 URA2 YPT31 HSP104 RPN7 TUB1 orf19.7297 ERG13 orf19.7328 UBC4 FAA4 FDH3 TRX1 XYL2 PHR2 SHM2 BMH1 YST1 RHO1 orf19.1833 RPL13 ERG6 HSP60 SRB1 ALO1 ANB1 ADE12 TSA1;TSA1B;TSA1B orf19.3061.1;RPS22A;orf19.3061.1 SEC4 CDC42 TEF2;TEF1 CYP1 CEF3 NMT1 ENO1 PMM1 RPS1 HSP70 PHR1 SEC14 PGK1 SSA2 HSP90 CDC19 GFA1 MET6 ACO1 GPM1 ACH1 ASC1 HXK2 IPP1 MDH1 PDC11 PGI1 POR1 QCR2 SAH1 SSC1 TIF MNT1 UCF1 UGP1 LSP1 URA6 PGA52 RPL3 TOM70 MCR1 VAC8 YHB1 ADE6 AAT21 orf19.3649 CBR1 GSP1 VMA2 ATP7 IMH3 TCP1 FUR1 DED81 orf19.6701 VPH1 ILS1 NOP5 SAR1 MIS11 MEU1 SAP9 RPS8A CYS4 RPL17B MRF1 GLK1;GLK4 DPS1-1 SIS1 orf19.3859 HHF1;HHF22 orf19.3681 GPD2 GAP4 CDC48 orf19.2335 orf19.86 GPX2 VPS21 GPD1 ACS1 MP65 YWP1 SSO2 orf19.1355 CCT7 CCT5 orf19.2244 ATP4 ERF1 TAL1 RNR21 EFT2 PDA1 SDH12 RPT1 GRS1 PRD1 YVC1 KRE30 VMA5 ERV25 RPS20 SSB1 SER33 RPN2 SEC23 SUR7 ADK1 FAS1 PET9 PRX1 ENA21 PDB1 SSZ1 RPL24A SEC26 SRV2 RPL15A ADE17 RPT4 TKL1 MLT1 RPS24 ALA1 orf19.3335 RPS21 CSP37 SUI2 DHH1 CCT8 RPL16A TUF1 QCR7 MXR1 HGT6 TDH3 TPD3 RPS12 KRS1 CCP1 RPL9B AHP1 EMP70 ZUO1 CRH11 RPS5 YNK1 GCD11 PRT1 LAT1 RPL5 PFK2 YIM1 YPT1 TPS2 orf19.3037 RLI1 YKT6 HOM6 SNZ1 RPL10 RPS7A TFP1 DBP5 RPL12 PGA4 CCT3 PFK1 URA7 orf19.3915 MYO2 PSA2 orf19.4931 RPS26A APT1 ARO1 NIP1 MDH1-1 ERV29 BGL2 CDR1;CDR2 PHB2 RDI1 NCE102 orf19.4898 MIR1 MLS1 MTS1 GUA1 COX5 SEC24 ACS2 TPS1 HSP78 MSI3 ATP6 COX2 SES1 SEC61 TPI1 FBA1 RPL10A OBPA</t>
+          <t>UBP6 TUB2 orf19.3341 RPS4A;RPS42 HGT1 orf19.3690.2 GSC1 FRS2 RPS16A RPL6 ECM33 CDC12 RPN3 orf19.1054 CDC3 ATP1 PIL1 SEC21 YBN5 orf19.2478.1 orf19.2489 RPS14B orf19.6264.3 RPS23A RAC1 ADE5,7 orf19.1229 DPM1 orf19.5085 DAK2 IDH1 ERO1 RPS17B RPL2 SAM2 GAD1 orf19.5281 RPL27A PEP1 CHS3 RPN1 RPL14 SEC18 ACT1 orf19.5006.1 GND1 RPL4B GDI1 HGT7 KAR2 orf19.1993 PLB4.5 MSB2 ARO3 orf19.1564 IDH2 ALD5 LHS1 RPL21A RPS9B RPL39 ERG10 RHO3 CYT1 orf19.6883 orf19.6882.1 COX9 VAS1 RPL11 GDH2 RPS10 PHM7 orf19.2175 orf19.2168.3 RPT6 ASN1 PMA1 KGD1 ARF3 orf19.1672 RNA1 RIP1 orf19.5917.3 RPS15 RPL35 RPL19A RPL18 RPS19A FAS2 YCK2 CAM1 UBA1 LYS9 CYP5 orf19.6741 FUM12 SUB2 PRO3 ATP2 CAR2 RPS6A RPL20B IDI1 orf19.2720 NCP1 RPN6 PYC2 orf19.1409.1 orf19.3799 RPL30 LYS1 TRP5 GDH3 CCT6 GUT2 RPT5 orf19.5682 THS1 VPS1 orf19.4149.1 orf19.4246 CAM1-1 RPS25B RPL43A MES1 ADH1 orf19.4016 HET1 FET34 RPS13 ILV5 RPL32 RPL25 CHC1 RPL23A SAC6 orf19.5627 GUS1 GLN4 GPH1 RPS18 RPP0 orf19.6507 PDI1 SHM1 SUI3 YRB1 ACC1 CRM1 ATP3 CDC60 FRS1 VMA4 ADH5 ECM4 IDP2 RPL28 ARC1 IFR2 CIT1 PRE6 RPS3 VMA13 GLN1 PST3 YCP4 LSC2 URA2 YPT31 HSP104 RPN7 TUB1 orf19.7297 ERG13 orf19.7328 UBC4 FAA4 FDH3 TRX1 XYL2 PHR2 SHM2 BMH1 YST1 RHO1 orf19.1833 RPL13 ERG6 HSP60 SRB1 ALO1 ANB1 ADE12 TSA1;TSA1B;TSA1B orf19.3061.1;RPS22A;orf19.3061.1 SEC4 CDC42 TEF2;TEF1 CYP1 CEF3 NMT1 ENO1 PMM1 RPS1 HSP70 PHR1 SEC14 PGK1 SSA2 HSP90 CDC19 GFA1 MET6 ACO1 GPM1 ACH1 ASC1 HXK2 IPP1 MDH1 PDC11 PGI1 POR1 QCR2 SAH1 SSC1 TIF MNT1 UCF1 UGP1 LSP1 URA6 PGA52 RPL3 TOM70 MCR1 VAC8 YHB1 ADE6 AAT21 orf19.3649 CBR1 GSP1 VMA2 ATP7 IMH3 TCP1 FUR1 DED81 orf19.6701 VPH1 ILS1 NOP5 SAR1 MIS11 MEU1 SAP9 RPS8A CYS4 RPL17B MRF1 GLK1;GLK4 DPS1-1 SIS1 orf19.3859 HHF1;HHF22 orf19.3681 GPD2 GAP4 CDC48 orf19.2335 orf19.86 VPS21 GPD1 ACS1 MP65 YWP1 SSO2 orf19.1355 CCT7 CCT5 orf19.2244 ATP4 ERF1 TAL1 RNR21 EFT2 PDA1 SDH12 RPT1 GRS1 PRD1 KRE30 VMA5 ERV25 RPS20 SSB1 SER33 RPN2 SEC23 SUR7 ADK1 FAS1 PET9 PRX1 ENA21 PDB1 SSZ1 RPL24A SEC26 SRV2 RPL15A ADE17 RPT4 TKL1 MLT1 RPS24 ALA1 orf19.3335 RPS21 CSP37 SUI2 DHH1 CCT8 RPL16A TUF1 QCR7 MXR1 HGT6 TDH3 TPD3 RPS12 KRS1 CCP1 RPL9B AHP1 EMP70 ZUO1 CRH11 RPS5 YNK1 GCD11 PRT1 LAT1 RPL5 PFK2 YIM1 YPT1 TPS2 orf19.3037 RLI1 YKT6 HOM6 SNZ1 RPL10 RPS7A TFP1 DBP5 RPL12 PGA4 CCT3 PFK1 URA7 orf19.3915 MYO2 PSA2 orf19.4931 RPS26A APT1 ARO1 NIP1 MDH1-1 ERV29 BGL2 CDR1;CDR2 PHB2 RDI1 NCE102 orf19.4898 MIR1 MLS1 MTS1 GUA1 COX5 SEC24 ACS2 TPS1 HSP78 MSI3 COX2 SES1 SEC61 TPI1 FBA1 RPL10A OBPA</t>
         </is>
       </c>
     </row>
@@ -443,11 +443,11 @@
         </is>
       </c>
       <c r="F3">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>MVD GGA2 orf19.3053 RIB4 orf19.6220.4 LTP1 SAM4 ZWF1 KEX2 orf19.4805 DOA1 orf19.6358 YPT52 orf19.7269 ATP18 orf19.1514 HPT1 UGA1 ERG20 orf19.4127 AAT1 TPS3 TOS1 LAP41 BAT22 FBP1 HIS4 HRT2 orf19.4609 TRP4 COF1 orf19.4153 RET2 UAP1 SCW11 ARD EBP1 SEC27 ADO1 GLC3 orf19.1212 orf19.2124 GLE2 orf19.6559 orf19.5184 orf19.7199 SLA2 orf19.7531 ADE1 ARC19 TRP2 URA5 PGM2 orf19.4395 ADE13 RPS27 ARO2 CHS2 orf19.7306 ARP2 PLB3 AHA1 CDC11 TUP1 CBP1 PMI1 CDC10 MNT2 CYC1 ARO4 GRP2 VMA8 orf19.3515 APE2 ALS3 HEM13 GLC7 BUD7 HSM3 LPD1 orf19.3459 OSM1 RBT1 MET15 orf19.1057 SEP7 CCS1 PHO15 orf19.2304 RAS1 RSP5 CCT2 orf19.1394 SUP35 orf19.3129 CDC68 orf19.1946 CYS3 WRS1 RIB3 orf19.3442 PFY1 GSY1 orf19.3235 orf19.3319 ARC35 SVF1 orf19.6065 PRO2 TIP120 orf19.338 GRX3 TYS1 TRR1 orf19.4248 orf19.891 ENG1 AGM1 HYR1 orf19.4633 POL30 SBP1 SFH5 HOG1 EIF4E</t>
+          <t>MVD GGA2 orf19.3053 RIB4 orf19.6220.4 LTP1 SAM4 ZWF1 orf19.4805 DOA1 orf19.6358 orf19.7269 ATP18 orf19.1514 HPT1 UGA1 ERG20 orf19.4127 AAT1 TPS3 TOS1 LAP41 BAT22 FBP1 HIS4 HRT2 orf19.4609 TRP4 COF1 orf19.4153 RET2 UAP1 SCW11 ARD EBP1 SEC27 ADO1 GLC3 orf19.1212 GLE2 orf19.6559 orf19.5184 orf19.7199 SLA2 orf19.7531 ADE1 ARC19 TRP2 URA5 PGM2 orf19.4395 ADE13 RPS27 ARO2 CHS2 orf19.7306 ARP2 PLB3 AHA1 CDC11 TUP1 CBP1 PMI1 CDC10 MNT2 CYC1 ARO4 GRP2 VMA8 orf19.3515 APE2 ALS3 HEM13 GLC7 BUD7 HSM3 LPD1 orf19.3459 OSM1 RBT1 MET15 orf19.1057 SEP7 CCS1 PHO15 orf19.2304 RAS1 RSP5 CCT2 orf19.1394 SUP35 orf19.3129 orf19.1946 CYS3 WRS1 RIB3 orf19.3442 PFY1 GSY1 orf19.3235 orf19.3319 ARC35 SVF1 orf19.6065 PRO2 TIP120 orf19.338 GRX3 TYS1 TRR1 orf19.4248 orf19.891 ENG1 AGM1 HYR1 orf19.4633 POL30 SBP1 SFH5 HOG1 EIF4E</t>
         </is>
       </c>
     </row>
@@ -470,11 +470,11 @@
         </is>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>IST2 PST1 POX1-3</t>
+          <t>PST1 GPX2 YVC1 POX1-3</t>
         </is>
       </c>
     </row>
@@ -497,11 +497,11 @@
         </is>
       </c>
       <c r="F5">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>PLB5 PNG2 ARA1 LEU42 orf19.1785 PNP1 PUP3 PRE5 ARG1 RSR1 CAT1 RBP1 CHT2 SAP5 RVS167 orf19.3508 orf19.1796 SOL3 EMP24 SPE3 SOD5 orf19.6816 GST2 YPS7</t>
+          <t>PLB5 YPT52 PNG2 ARA1 LEU42 orf19.1785 PNP1 orf19.2124 PUP3 PRE5 ARG1 RSR1 CAT1 RBP1 CHT2 SAP5 RVS167 orf19.3508 orf19.1796 SOL3 EMP24 SPE3 CDC68 SOD5 orf19.6816 GST2 YPS7</t>
         </is>
       </c>
     </row>
@@ -524,11 +524,11 @@
         </is>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>ARO8 RPT2 LEU2 VTC3 VTC4 FDH1 COI1 PGA63 NDE1 MET3</t>
+          <t>orf19.6066 orf19.1152 ARO8 RPT2 VMA6 orf19.3983 LEU2 VTC3 VTC4 FDH1 COI1 PGA63 NDE1 ATP6 MET3</t>
         </is>
       </c>
     </row>
@@ -551,11 +551,11 @@
         </is>
       </c>
       <c r="F7">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>LYS2 orf19.5095 orf19.1444 orf19.6160 orf19.5671 HOM3 RIB5 SBA1 orf19.7086 CRN1 AHP2 orf19.6305 ARC40 SER1 HMO1 orf19.3679 ARP3 TFS1 orf19.1267 GVP36 orf19.933 FUM11 orf19.5393 MET2 PRN4 SLK19 HTA3 SEC13 GLX3 HSP21 PDX1 orf19.4953 MCA1 URE2 BCY1</t>
+          <t>LYS2 orf19.5095 KEX2 orf19.1444 orf19.6160 orf19.5671 HOM3 RIB5 SBA1 orf19.7086 CRN1 AHP2 orf19.6305 ARC40 SER1 HMO1 orf19.3679 ARP3 TFS1 orf19.1267 GVP36 orf19.933 FUM11 orf19.5393 MET2 PRN4 SLK19 HTA3 SEC13 GLX3 HSP21 PDX1 orf19.4953 MCA1 URE2 BCY1</t>
         </is>
       </c>
     </row>
@@ -578,11 +578,11 @@
         </is>
       </c>
       <c r="F8">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>orf19.2988 orf19.5054 orf19.1840 FMP45 YCF1 ADP1 SLP3 orf19.7310 orf19.2163 HTA1 APR1 SIM1</t>
+          <t>orf19.2988 IST2 orf19.5054 orf19.1840 FMP45 YCF1 ADP1 SLP3 orf19.7310 orf19.2163 HTA1 APR1 SIM1</t>
         </is>
       </c>
     </row>
@@ -632,11 +632,11 @@
         </is>
       </c>
       <c r="F10">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>orf19.6082 RPS21B orf19.2954 HMG1 SSH1 orf19.2460 GLT1 orf19.4758 SAC1 orf19.2328 WBP1 ERP5 GAR1 RPL38 orf19.1549 orf19.1578 TOM1 COX6 QCR8 orf19.3572.3 ECM17 orf19.2257 TIF4631 GCN1 FOX2 ALI1 orf19.1682 ILV2 PHB1;orf19.357 CTP1 OST1 NOG1 STE24 orf19.5660.1 ERG251 EFB1 orf19.3810 orf19.3782.2 orf19.1956 orf19.4131 THR4 orf19.1179 YHM1 orf19.5516 SNQ2 orf19.1086 orf19.7011 HHO1 MIS12 ATP17 PCK1 MRPL6 RPS30 SEC63 YDJ1 orf19.3518 orf19.6119 orf19.6415.1 PHO88 NUO1 MSS51 SIK1 orf19.7590 ERG5 PMT1 ADH2 COX1 ERG11 orf19.1052;HTB1 ATP20 orf19.51 YHM2 RPG1A SPF1 KTR4 SDH2 GNP1 PTR22 orf19.6887 orf19.4517 NDH51 HEM15 LYS21 orf19.1030 HGT2 TIM50 YMC1 ALP1 FAD2 orf19.2286 orf19.3558 SUR2 PR26 RNR1 NOP1 UBI3;UBI4 orf19.7459 orf19.1239 DED1 orf19.3430 MET14 SCS7 SDS24 OLE1 FUN12 RHR2 ATP5 IFF11 ERG27 LSC1 PGA45 CHT1 orf19.6035 orf19.5517 CPR6 RFA1 orf19.2017 PMT2 NUO2 orf19.6565 NUC2 TOM40 orf19.1691 orf19.3994 HAS1 SSD1 orf19.1480 STT3 COX4 COX13 orf19.4706 BFR1 RPL8B ARF2 URA1 GDA1 ERG1 ADE2 NAD5 RPP1A</t>
+          <t>orf19.6082 RPS21B orf19.2954 HMG1 SSH1 orf19.2460 GLT1 orf19.4758 SAC1 orf19.2328 WBP1 ERP5 RPL38 orf19.1549 orf19.1578 TOM1 COX6 QCR8 orf19.3572.3 ECM17 orf19.2257 TIF4631 GCN1 FOX2 ALI1 orf19.1682 ILV2 PHB1;orf19.357 OST1 STE24 orf19.5660.1 ERG251 EFB1 orf19.3810 orf19.3782.2 orf19.1956 THR4 orf19.1179 YHM1 orf19.5516 SNQ2 orf19.1086 orf19.7011 HHO1 PCK1 MRPL6 RPS30 SEC63 YDJ1 orf19.6119 orf19.6415.1 PHO88 NUO1 MSS51 SIK1 orf19.7590 ERG5 PMT1 ADH2 COX1 ERG11 orf19.1052;HTB1 ATP20 orf19.51 RPG1A SPF1 KTR4 SDH2 GNP1 PTR22 orf19.6887 orf19.4517 NDH51 LYS21 orf19.1030 TIM50 YMC1 ALP1 FAD2 orf19.2286 orf19.3558 SUR2 PR26 RNR1 NOP1 UBI3;UBI4 orf19.1239 DED1 orf19.3430 MET14 SCS7 SDS24 OLE1 FUN12 RHR2 ATP5 IFF11 ERG27 LSC1 PGA45 CHT1 orf19.6035 orf19.5517 CPR6 RFA1 PMT2 NUO2 NUC2 TOM40 SSD1 orf19.1480 COX4 COX13 orf19.4706 BFR1 RPL8B ARF2 URA1 GDA1 ERG1 ADE2 RPP1A</t>
         </is>
       </c>
     </row>
@@ -659,11 +659,11 @@
         </is>
       </c>
       <c r="F11">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>GAL10 AGE3 orf19.2930 DIP5 orf19.71 orf19.5194.1 FMA1 orf19.2439.1 LHP1 CDR4 GCR3 ARG5,6 ERG12 GCA2;GCA1 CTA3 orf19.5274 SPA2 RBK1 OP4 MUQ1 orf19.2095 orf19.1533 ADE8 orf19.5783 HEM2 DCK1 TAF14 RIM11;orf19.792 RPC40 orf19.6867 FRP3 RNR22 ERG9 SGT1 PUS7 FLO9 orf19.158 PPT1 orf19.1655.3 orf19.1626 APL2 orf19.5943.1 CHS4 orf19.7357 orf19.7368 orf19.6787 orf19.6189 orf19.5665 orf19.2757 orf19.3792 OFD1 orf19.3124 orf19.5689 AFL1 orf19.581 orf19.3185 orf19.4228 TIF5 CAR1 RPN5 HOC1 DOG1 PLB2 orf19.5525 APA2 SNF4 RPS28B LMO1 GYP7 orf19.7198 NPT1 orf19.7485 NTH1 orf19.2520 IFE2 ACO2 FLC2 EMP46 KGD2 RPP2A orf19.7322 BET2 orf19.2965 orf19.6676;orf19.1124.2 SAP3 CHT3 CDC28 SPT6 orf19.1815 SUI1 DBP2 ARO10 orf19.6284 HAM1 PUP2 orf19.399 MNN26 NMD5 ARO7 orf19.5669 RAD51 ERG3 HTA2 PHO100 MNN2 ARC18 orf19.4107 RPN10 orf19.1782 orf19.2246 TIF35 orf19.4382 orf19.4375 orf19.7153 SER2 orf19.3136 orf19.2426 AQY1 orf19.5229 MDH1-3 RHD3 orf19.5293 DRG1 GLO3 TMA19 LAG1 orf19.3312 HMT1 orf19.2518 NPL4 NAP1 PHHB MNN24 orf19.6804 HHT1;HHT2;HHT21 orf19.6748 SLC1 SAP8 RVB2 SDS22 orf19.3045 SEC62 TIF34 TOM20 CDC53 UTR2 HTS1 ILV3 orf19.4960 SPT5 RAT1 HGH1 orf19.5965 PKC1 orf19.5885 EGD2 orf19.4850 DBP3 SSU81 THR1 PLB1</t>
+          <t>GAL10 AGE3 orf19.2930 DIP5 orf19.71 orf19.5194.1 FMA1 LHP1 CDR4 GCR3 ARG5,6 ERG12 GCA2;GCA1 CTA3 RBK1 orf19.2095 orf19.1533 ADE8 orf19.5783 HEM2 TAF14 RIM11;orf19.792 RPC40 orf19.6867 FRP3 RNR22 ERG9 SGT1 FLO9 orf19.158 PPT1 orf19.1655.3 orf19.1626 orf19.5943.1 CHS4 orf19.7357 orf19.7368 orf19.6787 orf19.6189 orf19.5665 orf19.2757 orf19.3792 OFD1 orf19.3124 orf19.5689 AFL1 orf19.581 orf19.3185 orf19.4228 TIF5 CAR1 RPN5 HOC1 DOG1 orf19.5525 APA2 SNF4 RPS28B LMO1 orf19.7198 NPT1 orf19.7485 NTH1 orf19.2520 IFE2 ACO2 FLC2 KGD2 RPP2A orf19.7322 BET2 orf19.2965 orf19.6676;orf19.1124.2 CHT3 orf19.1815 SUI1 DBP2 ARO10 HAM1 PUP2 MNN26 ARO7 orf19.5669 RAD51 ERG3 HTA2 ARC18 orf19.4107 RPN10 orf19.1782 orf19.2246 TIF35 orf19.4382 orf19.7153 SER2 orf19.2426 orf19.5229 MDH1-3 orf19.5293 DRG1 GLO3 TMA19 LAG1 orf19.3312 HMT1 orf19.2518 NAP1 PHHB MNN24 orf19.6804 HHT1;HHT2;HHT21 orf19.6748 SLC1 SAP8 RVB2 SDS22 orf19.3045 SEC62 TIF34 TOM20 CDC53 UTR2 HTS1 ILV3 orf19.4960 HGH1 PKC1 orf19.5885 EGD2 orf19.4850 DBP3 SSU81 THR1 PLB1</t>
         </is>
       </c>
     </row>
@@ -686,11 +686,11 @@
         </is>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>SFC1 orf19.7307 ICL1 orf19.2484 orf19.3060</t>
+          <t>orf19.4131 SFC1 ATP17 orf19.3518 orf19.7307 ICL1 orf19.2484 orf19.3060</t>
         </is>
       </c>
     </row>
@@ -713,11 +713,11 @@
         </is>
       </c>
       <c r="F13">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>SNO1 CRP1 orf19.4952.1 orf19.4955 AGO1 orf19.577 HEX1 orf19.6553 APL4 MAL2 FLU1;TPO2 SAP2 MYO5 orf19.6423 MNN22 ALS1 orf19.6200 orf19.5611 orf19.2059 GCD2 DFI1 SSR1 MNN1 ECM331 orf19.1709 MAL31 PHO114 MNN12 LIP4</t>
+          <t>SNO1 CRP1 OP4 orf19.4955 DCK1 APL2 AGO1 orf19.577 HEX1 PLB2 orf19.6553 GYP7 APL4 MAL2 FLU1;TPO2 SAP3 SAP2 MYO5 PHO100 MNN2 orf19.6423 RHD3 MNN22 ALS1 NPL4 orf19.6200 orf19.5611 orf19.2059 GCD2 DFI1 SSR1 MNN1 ECM331 orf19.1709 MAL31 PHO114 MNN12 LIP4</t>
         </is>
       </c>
     </row>
@@ -740,11 +740,11 @@
         </is>
       </c>
       <c r="F14">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>orf19.3293 NEP1 PHO84 CSI2 orf19.2091 ENT3 DNM1 orf19.6828.1 orf19.2917 orf19.5698 orf19.1967 SEC8 CIC1 orf19.5547 orf19.6458.1 RPP1B orf19.7672 COB MNN9 NOC2 NMD3 orf19.409 orf19.397 orf19.213 orf19.4396 orf19.2821 PMT6 orf19.512 orf19.5077 BNA4 ZPR1 DRS1 COQ6 ARX1 OSM2 orf19.5991 MAK21 MSS116</t>
+          <t>orf19.3293 NEP1 PHO84 GAR1 CSI2 orf19.2091 ENT3 CTP1 DNM1 NOG1 orf19.6828.1 orf19.2917 orf19.5698 orf19.1967 SEC8 CIC1 orf19.5547 orf19.6458.1 RPP1B MIS12 orf19.7672 COB MNN9 NOC2 YHM2 NMD3 orf19.409 orf19.397 orf19.213 HEM15 HGT2 orf19.4396 orf19.2821 orf19.7459 PMT6 orf19.512 orf19.5077 BNA4 ZPR1 DRS1 orf19.2017 orf19.6565 COQ6 ARX1 orf19.1691 orf19.3994 HAS1 OSM2 STT3 orf19.5991 MAK21 MSS116 NAD5</t>
         </is>
       </c>
     </row>
@@ -767,11 +767,11 @@
         </is>
       </c>
       <c r="F15">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>RPO41 orf19.3304 orf19.3333 MRP20 GAL7 ROA1 orf19.2964 PDE2 MAS1 orf19.3027 EHT1 NOP4 PHO85 orf19.6843 orf19.6853 orf19.2485 TRP99 PHO87 orf19.6245 orf19.6259 orf19.4437;ISW2 ADE4 SMI1 GCS1 orf19.989 DJP1 orf19.2333 RPL82 orf19.2330 orf19.1139 TRP3 orf19.6355 KEM1 NPL3 orf19.7234 RPC10 DDI1 orf19.7264 orf19.2019 orf19.1516 UTP22 orf19.5834 UTP21 orf19.880 GCD7 orf19.804.1 BAT21 orf19.4488 orf19.185 orf19.3547 orf19.3552 orf19.3556 orf19.3559 orf19.3583 orf19.2228 orf19.2278 orf19.1889 MCM3 orf19.2165 SLP2 orf19.1389 MET10 FCY21 orf19.1404 orf19.1381 YOR1 CHS8 UTP20 GEA2 orf19.1697 orf19.1662 UTP4 AIP2 KRE5 KRE6 PBS2 orf19.7404 orf19.6828 NUP159 orf19.6718 PTC7 HIS5 orf19.4686 PWP1 ILV6 orf19.2755 orf19.2686 MSN5 orf19.2664 orf19.3367 RRP42 orf19.1791 orf19.1272 orf19.3141 orf19.3128 orf19.1961 SNF1 MAS2 STI1 RPN8 orf19.3183 orf19.6665 orf19.2639.1 GUK1 MTR10 orf19.3914 orf19.4030 orf19.4029 FCA1 orf19.4193 TIF3 HCH1 orf19.688 orf19.3480 NIP7 GCV1 NAB3 orf19.5541 POL5 orf19.5607 NOG2 orf19.5747 NUP82 orf19.73 CDC39 orf19.1085 orf19.2143 orf19.2150 orf19.7108 orf19.7097 orf19.7069 orf19.7088 PEL1 RPA135 orf19.7067 NOP15 YML6 orf19.7012 GCN3 orf19.2371 POL3 orf19.2372 orf19.5161 orf19.1338 orf19.1335 ENP1 orf19.7197 MRP7 MAM33 KAP120 orf19.7160 orf19.7152 orf19.7522 LEU1 orf19.7478 PTC2 SHP1 orf19.2820 PAN6 orf19.2835 orf19.501 PDX3 orf19.639.1 RGD3;orf19.730 orf19.7290 orf19.7326 ELF1 orf19.6612 YKE2 orf19.6597 CTM1 RFC4 RPO21 HEM3 MRPS9 NSA2;orf19.7397.1;orf19.7397.1;orf19.7398 CDC21 URA3 MEX67 SPL1 IPK1 SIT4 orf19.1214 orf19.3755 orf19.5206 orf19.1849 orf19.4204 ILV1 orf19.6346 SDA1 RTS1 GCF1 orf19.394 CAF16 orf19.4479 ARC15 MRPL8 DBP7 orf19.3477 orf19.3463 CCC1 orf19.6868 orf19.4537 orf19.1305 orf19.1304 orf19.1162 EGD1 PPZ1 RPL7 ERB1 SKP1 orf19.2352 UBA4 PES1 EFG1 IMP4 orf19.585 UTP15 orf19.3585 TIM23 orf19.2275 RFA2 AAH1 RPF2 MRPL10 CKA2 orf19.7215 orf19.4373 MCM2 orf19.5812 PLC2;FGR22 orf19.2920 orf19.1970 orf19.439 PRS5 orf19.6424 TSR1 orf19.5235 orf19.7291 orf19.1248 orf19.3446 orf19.969 NAM7 orf19.5168 orf19.5356 LYS4 MRP8 orf19.3836 orf19.3798 orf19.3797 orf19.547 orf19.498 MRPL3 TIM44 orf19.5442 orf19.5420 PBP2 SKI8 orf19.5757 HGT10 orf19.3357 orf19.3349 MBF1 SEC65 LYS12 ARP9 orf19.2438 MRPL19 KEL1 orf19.6090 CNS1 MRT4 orf19.5515 ARP4 orf19.7546 NDT80 orf19.2008 orf19.6822 SSN6 MET8 orf19.6752 orf19.6717 UTP9 ABP1 orf19.4340 orf19.4306 orf19.4283 GIR2 EXO70 orf19.6503 orf19.863 orf19.3022 orf19.1687 orf19.1646 orf19.4021 orf19.4018 orf19.3977 orf19.4932 PRS1 orf19.1565 HOM2 CPR3 orf19.1545 orf19.4611 orf19.4597 CAT2 orf19.5989 orf19.5961 YTM1 orf19.4751 HBR1 CDC37</t>
+          <t>RPO41 orf19.3304 orf19.3333 MRP20 GAL7 ROA1 orf19.2964 PDE2 orf19.3027 EHT1 NOP4 PHO85 orf19.6843 orf19.6853 orf19.2485 TRP99 orf19.2439.1 PHO87 orf19.6245 orf19.6259 orf19.4437;ISW2 ADE4 SMI1 GCS1 orf19.989 DJP1 orf19.2333 RPL82 orf19.2330 orf19.1139 orf19.5274 TRP3 orf19.6355 SPA2 KEM1 NPL3 orf19.7234 RPC10 DDI1 orf19.7264 MUQ1 orf19.2019 orf19.1516 UTP22 orf19.5834 UTP21 orf19.880 GCD7 orf19.804.1 BAT21 orf19.4488 orf19.185 orf19.3547 orf19.3552 orf19.3556 orf19.3559 orf19.3583 orf19.2228 orf19.2278 orf19.1889 MCM3 orf19.2165 SLP2 orf19.1389 MET10 FCY21 orf19.1404 orf19.1381 YOR1 PUS7 CHS8 UTP20 GEA2 orf19.1697 orf19.1662 UTP4 AIP2 KRE5 KRE6 PBS2 orf19.7404 orf19.6828 NUP159 orf19.6718 PTC7 HIS5 orf19.4686 PWP1 ILV6 orf19.2755 orf19.2686 MSN5 orf19.2664 orf19.3367 RRP42 orf19.1791 orf19.1272 orf19.3141 orf19.3128 orf19.1961 SNF1 MAS2 STI1 RPN8 orf19.3183 orf19.6665 orf19.2639.1 GUK1 MTR10 orf19.3914 orf19.4030 orf19.4029 FCA1 orf19.4193 TIF3 HCH1 orf19.688 orf19.3480 NIP7 GCV1 NAB3 orf19.5541 POL5 orf19.5607 NOG2 orf19.5747 NUP82 orf19.73 CDC39 orf19.1085 orf19.2143 orf19.2150 orf19.7108 orf19.7097 orf19.7069 orf19.7088 PEL1 RPA135 orf19.7067 NOP15 YML6 orf19.7012 GCN3 orf19.2371 POL3 orf19.2372 orf19.5161 orf19.1338 orf19.1335 ENP1 orf19.7197 MRP7 MAM33 KAP120 orf19.7160 orf19.7152 orf19.7522 LEU1 orf19.7478 PTC2 SHP1 orf19.2820 PAN6 orf19.2835 orf19.501 PDX3 orf19.639.1 EMP46 RGD3;orf19.730 orf19.7290 orf19.7326 ELF1 orf19.6612 YKE2 orf19.6597 RFC4 RPO21 HEM3 MRPS9 NSA2;orf19.7397.1;orf19.7397.1;orf19.7398 CDC21 URA3 CDC28 MEX67 SPL1 SPT6 IPK1 SIT4 orf19.1214 orf19.3755 orf19.5206 orf19.1849 orf19.6284 orf19.4204 ILV1 orf19.6346 SDA1 RTS1 GCF1 orf19.399 orf19.394 CAF16 orf19.4479 ARC15 MRPL8 DBP7 orf19.3477 orf19.3463 NMD5 CCC1 orf19.6868 orf19.4537 orf19.1305 orf19.1304 orf19.1162 EGD1 PPZ1 RPL7 ERB1 SKP1 orf19.2352 UBA4 PES1 EFG1 IMP4 orf19.585 UTP15 orf19.3585 TIM23 orf19.2275 RFA2 AAH1 RPF2 MRPL10 CKA2 orf19.7215 orf19.4375 orf19.4373 MCM2 orf19.5812 PLC2;FGR22 orf19.3136 orf19.2920 orf19.1970 AQY1 orf19.439 orf19.6424 TSR1 orf19.5235 orf19.7291 orf19.1248 orf19.969 NAM7 orf19.5168 orf19.5356 LYS4 MRP8 orf19.3836 orf19.3798 orf19.3797 orf19.547 orf19.498 MRPL3 TIM44 orf19.5442 orf19.5420 PBP2 SKI8 orf19.5757 HGT10 orf19.3357 orf19.3349 MBF1 SEC65 LYS12 ARP9 orf19.2438 MRPL19 KEL1 orf19.6090 CNS1 MRT4 orf19.5515 ARP4 orf19.7546 NDT80 orf19.2008 orf19.6822 SSN6 MET8 orf19.6752 orf19.6717 UTP9 ABP1 orf19.4340 orf19.4306 orf19.4283 GIR2 EXO70 orf19.6503 orf19.863 orf19.3022 orf19.1687 orf19.1646 orf19.4021 orf19.4018 orf19.3977 orf19.4932 PRS1 orf19.1565 HOM2 CPR3 orf19.1545 SPT5 RAT1 orf19.4611 orf19.4597 CAT2 orf19.5989 orf19.5965 orf19.5961 YTM1 orf19.4751 HBR1 CDC37</t>
         </is>
       </c>
     </row>
@@ -871,11 +871,11 @@
         </is>
       </c>
       <c r="F2">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>MVD UBP6 TUB2 RPS21B orf19.3341 RPS4A;RPS42 GAL10 orf19.3690.2 GSC1 FRS2 RPS16A RPL6 ECM33 CDC12 orf19.3053 RPN3 CDC3 ATP1 PIL1 SEC21 YBN5 orf19.449 RIB4 orf19.2478.1 orf19.2489 TRP99 RPS14B RPS23A MMD1 LHP1 orf19.5054 ADE5,7 orf19.1229 LTP1 GCV2 DPM1 orf19.5085 ZWF1 DAK2 DOA1 IDH1 RPS17B RPL2 orf19.2296 SAM2 GAD1 orf19.5281 TRP3 RPL27A RPN1 RPL14 SEC18 ACT1 GND1 orf19.7215.3 RPL4B orf19.7214 GDI1 orf19.7269 orf19.7263 RPL38 ARO8 KAR2 orf19.1993 orf19.1514 ARO3 orf19.1564 HPT1 IDH2 ALD5 LHS1 RPL21A RPS9B RPL39 TAF14 ERG10 UGA1 ERG20 CYT1 AAT1 orf19.3572.3 orf19.6883 orf19.6882.1 IDP1 COX9 VAS1 PST1 orf19.1889 RPL11 GDH2 RPS10 orf19.2175 ARA1 orf19.2168.3 RPT6 ASN1 LEU42 TPS3 RPT2 ETR1 PMA1 orf19.6160 SCL1 KGD1 orf19.1672 RNA1 LAP41 ILV2 PNP1 RIP1 orf19.5917.3 RPS15 RPL35 RPL19A RPL18 RPS19A FAS2 orf19.5943.1 BAT22 CAM1 UBA1 LYS9 CYP5 FUM12 FBP1 VMA6 HIS4 SUB2 PRO3 ATP2 CAR2 RPS6A ILV6 HRT2 RPL20B orf19.4609 IDI1 orf19.2755 orf19.2720 NCP1 RPN6 PYC2 EFB1 orf19.1409.1 orf19.3799 RPL30 LYS1 XKS1 HOM3 NIF3 TRP5 GDH3 CCT6 OYE32 RPT5 orf19.5689 orf19.5682 THS1 COF1 VPS1 orf19.4149.1 STI1 orf19.4230 orf19.4246 TIF5 UAP1 THR4 GRE3 CAM1-1 RPS25B RPL43A MES1 ADH1 orf19.4016 HET1 RPS13 ILV5 EBP1 RPL32 RPL25 CHC1 RPL23A SEC27 orf19.5525 SAC6 ADO1 orf19.5620 orf19.5627 GLC3 SBA1 orf19.5773 orf19.2125 orf19.2150 LEU2 GUS1 GLN4 RPS28B GPH1 RPS18 RPP0 PRE10 orf19.6559 CRN1 orf19.6507 orf19.5184 HHO1 PDI1 SHM1 PUP3 CPY1 orf19.7199 MAM33 PRE5 SUI3 orf19.7140 orf19.7531 MIS12 orf19.7522 ADE1 YRB1 ARG1 ACC1 CRM1 ARC19 ATP3 TRP2 URA5 CDC60 FRS1 VMA4 ADH5 ECM4 IDP2 PGM2 RPL28 ARC1 IFR2 CIT1 orf19.4395 PRE6 PDX3 RPS3 VMA13 GLN1 PST3 ADE13 ARC40 LSC2 URA2 KGD2 ARO2 HSP104 orf19.6415.1 RPN7 TUB1 orf19.7297 ERG13 ARP2 orf19.7328 orf19.6596 UBC4 FAA4 FDH3 TRX1 XYL2 CDC11 CAT1 SHM2 BMH1 YST1 RHO1 orf19.1833 RPL13 ERG6 HSP60 SRB1 ALO1 ANB1 ADE12 TSA1;TSA1B;TSA1B orf19.3061.1;RPS22A;orf19.3061.1 SEC4 TUP1 TEF2;TEF1 CYP1 CEF3 RBP1 NMT1 ENO1 PMM1 PMI1 CDC10 RPS1 HSP70 SEC14 PGK1 SSA2 HSP90 CDC19 CYC1 GFA1 ARO4 MET6 ACO1 GPM1 ACH1 ASC1 GRP2 HXK2 IPP1 MDH1 PDC11 PGI1 POR1 QCR2 SAH1 SSC1 TIF SOU1 MNT1 orf19.1433 orf19.3515 UCF1 UGP1 LSP1 APE2 orf19.1214 RPL3 TOM70 orf19.3508 MCR1 GDB1 HEM13 YHB1 ADE6 AAT21 GLC7 LKH1 orf19.3649 GLR1 CBR1 orf19.1796 GSP1 SER1 ILV1 HSM3 HMO1 VMA2 ATP7 PUP2 SOL3 IMH3 TCP1 CSH1 FDH1 FUR1 DED81 orf19.6701 ILS1 LPD1 SAR1 MIS11 MEU1 HTA1 OSM1 RPS8A CYS4 orf19.4517 LYS22 RPL17B MRF1 GLK1;GLK4 APR1 DPS1-1 MET15 SIS1 HHF1;HHF22 orf19.3681 CCS1 HNT1 CDC48 orf19.2335 orf19.2304 orf19.86 orf19.590 GPD1 ACS1 PST2 CCT2 SUP35 orf19.1355 CCT7 ARP3 CCT5 SPE3 orf19.2244 ATP4 ERF1 TAL1 RNR21 PR26 EFT2 orf19.3129 PDA1 SDH12 URA4 TFS1 orf19.1946 RPT1 GRS1 PRD1 KRE30 CYS3 RPS20 SSB1 SER33 RPN2 WRS1 RIB3 SEC23 GVP36 orf19.3442 ADK1 FAS1 MET14 PET9 PRX1 orf19.5369 TIF11 PDB1 SSZ1 RPL24A FUM11 SEC26 SRV2 RPL15A ADE17 RPT4 TKL1 PFY1 RPS24 ATP5 DOT5 GSY1 TMA19 ALA1 LSC1 SOD2 RPS21 MBF1 CSP37 LYS12 ARC35 PGA63 SUI2 DHH1 CCT8 RPL16A SVF1 orf19.6065 GLO1 TUF1 QCR7 CPR6 PHHB orf19.2047 MXR1 HGT6 orf19.6816 TDH3 TPD3 RPS12 PRO2 SLK19 GCY1 KRS1 PRE9 orf19.338 SEC13 CCP1 RPL9B GLX3 AMS1 AHP1 orf19.2737 ZUO1 ABP1 TYS1 GST2 RPS5 YNK1 TRR1 orf19.4248 GCD11 PRT1 LAT1 RPL5 PFK2 RVB2 HSP21 TPS2 orf19.3037 RLI1 orf19.2966 HOM6 SNZ1 RPL10 RPS7A TFP1 DBP5 POX1-3 RPL12 HTS1 CCT3 PFK1 URA7 orf19.3915 PDX1 AGM1 orf19.4953 PSA2 orf19.4931 HOM2 CPR3 RPS26A orf19.1460 APT1 ARO1 NIP1 orf19.4633 POL30 MDH1-1 CAT2 PHB2 RDI1 orf19.5961 EGD2 SBP1 orf19.4898 MIR1 MLS1 MTS1 GUA1 COX5 SEC24 ACS2 ADE2 TPS1 HSP78 MSI3 URE2 COX2 BCY1 SES1 SEC61 TPI1 EIF4E FBA1 RPL10A NHP6A OBPA MET3</t>
+          <t>MVD UBP6 TUB2 RPS21B orf19.3341 RPS4A;RPS42 GAL10 orf19.3690.2 GSC1 FRS2 RPS16A RPL6 ECM33 CDC12 orf19.3053 RPN3 CDC3 ATP1 PIL1 SEC21 YBN5 orf19.449 RIB4 orf19.2478.1 orf19.2489 TRP99 RPS14B RPS23A MMD1 LHP1 orf19.5054 ADE5,7 orf19.1229 LTP1 GCV2 DPM1 orf19.5085 ZWF1 DAK2 DOA1 IDH1 RPS17B RPL2 orf19.2296 SAM2 GAD1 orf19.5281 TRP3 RPL27A RPN1 RPL14 SEC18 ACT1 GND1 orf19.7215.3 RPL4B orf19.7214 GDI1 orf19.7269 orf19.7263 RPL38 ARO8 KAR2 orf19.1993 orf19.1514 ARO3 orf19.1564 HPT1 IDH2 ALD5 LHS1 RPL21A RPS9B RPL39 TAF14 ERG10 UGA1 ERG20 CYT1 AAT1 orf19.3572.3 orf19.6883 orf19.6882.1 IDP1 COX9 VAS1 PST1 orf19.1889 RPL11 GDH2 RPS10 orf19.2175 ARA1 orf19.2168.3 RPT6 ASN1 LEU42 TPS3 RPT2 ETR1 PMA1 orf19.6160 SCL1 KGD1 orf19.1672 RNA1 LAP41 ILV2 PNP1 RIP1 orf19.5917.3 RPS15 RPL35 RPL19A RPL18 RPS19A FAS2 orf19.5943.1 BAT22 CAM1 UBA1 LYS9 CYP5 FUM12 FBP1 HIS4 SUB2 PRO3 ATP2 CAR2 RPS6A ILV6 HRT2 RPL20B orf19.4609 IDI1 orf19.2755 orf19.2720 NCP1 RPN6 PYC2 EFB1 orf19.1409.1 orf19.3799 RPL30 LYS1 XKS1 HOM3 NIF3 TRP5 GDH3 CCT6 OYE32 RPT5 orf19.5689 orf19.5682 THS1 COF1 VPS1 orf19.4149.1 STI1 orf19.4230 orf19.4246 TIF5 UAP1 THR4 GRE3 CAM1-1 RPS25B RPL43A MES1 ADH1 orf19.4016 HET1 RPS13 ILV5 EBP1 RPL32 RPL25 CHC1 RPL23A SEC27 orf19.5525 SAC6 ADO1 orf19.5620 orf19.5627 GLC3 SBA1 orf19.5773 orf19.2125 orf19.2150 LEU2 GUS1 GLN4 RPS28B GPH1 RPS18 RPP0 PRE10 orf19.6559 CRN1 orf19.6507 orf19.5184 HHO1 PDI1 SHM1 PUP3 CPY1 orf19.7199 MAM33 PRE5 SUI3 orf19.7140 orf19.7531 orf19.7522 ADE1 YRB1 ARG1 ACC1 CRM1 ARC19 ATP3 TRP2 URA5 CDC60 FRS1 VMA4 ADH5 ECM4 IDP2 PGM2 RPL28 ARC1 IFR2 CIT1 orf19.4395 PRE6 PDX3 RPS3 VMA13 GLN1 PST3 ADE13 ARC40 LSC2 URA2 KGD2 ARO2 HSP104 orf19.6415.1 RPN7 TUB1 orf19.7297 ERG13 ARP2 orf19.7328 orf19.6596 UBC4 FAA4 FDH3 TRX1 XYL2 CDC11 CAT1 SHM2 BMH1 YST1 RHO1 orf19.1833 RPL13 ERG6 HSP60 SRB1 ALO1 ANB1 ADE12 TSA1;TSA1B;TSA1B orf19.3061.1;RPS22A;orf19.3061.1 SEC4 TUP1 TEF2;TEF1 CYP1 CEF3 RBP1 NMT1 ENO1 PMM1 PMI1 CDC10 RPS1 HSP70 SEC14 PGK1 SSA2 HSP90 CDC19 CYC1 GFA1 ARO4 MET6 ACO1 GPM1 ACH1 ASC1 GRP2 HXK2 IPP1 MDH1 PDC11 PGI1 POR1 QCR2 SAH1 SSC1 TIF SOU1 MNT1 orf19.1433 orf19.3515 UCF1 UGP1 LSP1 APE2 RPL3 TOM70 orf19.3508 MCR1 GDB1 HEM13 YHB1 ADE6 AAT21 GLC7 LKH1 orf19.3649 GLR1 CBR1 orf19.1796 GSP1 SER1 ILV1 HSM3 HMO1 VMA2 ATP7 PUP2 SOL3 IMH3 TCP1 CSH1 FDH1 FUR1 DED81 orf19.6701 ILS1 LPD1 SAR1 MIS11 MEU1 OSM1 RPS8A CYS4 orf19.4517 RPL17B MRF1 GLK1;GLK4 APR1 DPS1-1 MET15 SIS1 HHF1;HHF22 orf19.3681 CCS1 HNT1 CDC48 orf19.2335 orf19.2304 orf19.86 orf19.590 GPD1 ACS1 PST2 CCT2 SUP35 orf19.1355 CCT7 ARP3 CCT5 SPE3 orf19.2244 ATP4 ERF1 TAL1 RNR21 PR26 EFT2 orf19.3129 PDA1 SDH12 URA4 TFS1 orf19.1946 RPT1 GRS1 PRD1 KRE30 CYS3 RPS20 SSB1 SER33 RPN2 WRS1 RIB3 SEC23 GVP36 orf19.3442 ADK1 FAS1 MET14 PET9 PRX1 orf19.5369 TIF11 PDB1 SSZ1 RPL24A FUM11 SEC26 SRV2 RPL15A ADE17 RPT4 TKL1 PFY1 RPS24 ATP5 DOT5 GSY1 TMA19 ALA1 LSC1 SOD2 RPS21 MBF1 CSP37 LYS12 ARC35 PGA63 SUI2 DHH1 CCT8 RPL16A SVF1 orf19.6065 GLO1 TUF1 QCR7 CPR6 PHHB orf19.2047 MXR1 HGT6 orf19.6816 TDH3 TPD3 RPS12 PRO2 SLK19 GCY1 KRS1 PRE9 orf19.338 SEC13 CCP1 RPL9B GLX3 AMS1 AHP1 orf19.2737 ZUO1 ABP1 TYS1 GST2 RPS5 YNK1 TRR1 orf19.4248 GCD11 PRT1 LAT1 RPL5 PFK2 RVB2 HSP21 TPS2 orf19.3037 RLI1 orf19.2966 HOM6 SNZ1 RPL10 RPS7A TFP1 DBP5 POX1-3 RPL12 HTS1 CCT3 PFK1 URA7 orf19.3915 PDX1 AGM1 orf19.4953 PSA2 orf19.4931 HOM2 CPR3 RPS26A orf19.1460 APT1 ARO1 NIP1 orf19.4633 POL30 MDH1-1 CAT2 PHB2 RDI1 EGD2 SBP1 orf19.4898 MIR1 MLS1 MTS1 GUA1 COX5 SEC24 ACS2 ADE2 TPS1 HSP78 MSI3 URE2 COX2 BCY1 SES1 SEC61 TPI1 EIF4E FBA1 RPL10A NHP6A OBPA MET3</t>
         </is>
       </c>
     </row>
@@ -898,11 +898,11 @@
         </is>
       </c>
       <c r="F3">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>orf19.3689 LYS2 orf19.3003 orf19.2988 GGA2 orf19.71 LPG20 orf19.6220.4 orf19.2794 ARG5,6 ERG12 NTF2 orf19.6358 PEP1 RBK1 MDG1 orf19.7264 orf19.1444 DCK1 BAT21 orf19.6867 PNG2 GRE2 orf19.1860.1 PPH21 HAL3 orf19.4639 TRP4 HSP12;orf19.4216 RET2 orf19.6658 CAR1 RIB5 ARD HCH1 STE23 GLE2 orf19.7108 orf19.7086 AHP2 HIS7 SLA2 orf19.7196 orf19.7152 PTC2 SHP1 orf19.6305 YCP4 YPT31 RPS27 orf19.7306 PRE8 PUP1 CBP1 VMA8 URA6 SUI1 BUD7 BUB3 ARC15 orf19.3459 UGA2 orf19.1057 SEP7 GPD2 PHO15 NIT3 RPN10 RAS1 orf19.1394 orf19.2262 PRE2 SGT2 VMA5 orf19.6423 MAE1 orf19.933 LAP3 OFR1 orf19.5393 orf19.3235 orf19.3319 MET2 RIM1 TTR1 orf19.2036 orf19.2008 orf19.6809 TIP120 GRX3 orf19.891 YPT1 YKT6 PRE1 orf19.3922 MYO2 CDC55 MCA1 CDC37 HOG1</t>
+          <t>orf19.3689 LYS2 orf19.2988 GGA2 orf19.71 LPG20 orf19.6220.4 orf19.2794 ARG5,6 ERG12 NTF2 orf19.6358 PEP1 RBK1 MDG1 orf19.7264 orf19.1444 orf19.6867 PNG2 GRE2 orf19.1860.1 PPH21 orf19.4639 TRP4 HSP12;orf19.4216 RET2 orf19.6658 CAR1 RIB5 ARD HCH1 STE23 GLE2 orf19.7108 AHP2 SLA2 orf19.7152 PTC2 SHP1 orf19.6305 YCP4 YPT31 RPS27 orf19.7306 PRE8 PUP1 CBP1 VMA8 URA6 SUI1 BUD7 BUB3 ARC15 orf19.3459 UGA2 orf19.1057 SEP7 GPD2 PHO15 NIT3 RPN10 RAS1 orf19.1394 orf19.2262 PRE2 SGT2 VMA5 orf19.6423 MAE1 orf19.933 LAP3 OFR1 orf19.5393 orf19.3235 orf19.3319 MET2 RIM1 TTR1 orf19.2036 orf19.6809 TIP120 GRX3 orf19.891 YPT1 YKT6 PRE1 MYO2 CDC55 MCA1 CDC37 HOG1</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>orf19.5095 SAM4 ERO1 ARO9 CIP1 CRG1 orf19.715 ALS3 VMA10 VPS21 ARG3 RKI1 SFH5</t>
+          <t>SAM4 ERO1 DCK1 ARO9 CIP1 CRG1 orf19.715 ALS3 VMA10 VPS21 ARG3 RKI1 SFH5</t>
         </is>
       </c>
     </row>
@@ -979,11 +979,11 @@
         </is>
       </c>
       <c r="F6">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>orf19.6264.3 orf19.1152 orf19.5006.1 SOD3 orf19.3859 orf19.3335 orf19.3932 NCE102</t>
+          <t>orf19.6264.3 orf19.1152 orf19.5006.1 VMA6 SOD3 MIS12 orf19.1214 HTA1 LYS22 orf19.3859 orf19.3335 orf19.3932 orf19.5961 NCE102</t>
         </is>
       </c>
     </row>
@@ -1006,11 +1006,11 @@
         </is>
       </c>
       <c r="F7">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>IST2 orf19.7210 MUQ1 orf19.4127 ARF3 orf19.5671 HIS5 AHA1 GUT1 VPH1 orf19.3679 ERV25 orf19.1267 HTA3 orf19.2769</t>
+          <t>orf19.3003 IST2 orf19.7210 MUQ1 BAT21 orf19.4127 ARF3 HAL3 orf19.5671 HIS5 orf19.7086 HIS7 orf19.7196 AHA1 GUT1 VPH1 orf19.3679 ERV25 orf19.1267 orf19.2008 HTA3 orf19.2769 orf19.3922</t>
         </is>
       </c>
     </row>
@@ -1060,11 +1060,11 @@
         </is>
       </c>
       <c r="F9">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>orf19.6079 orf19.6066 orf19.4530.1 orf19.4476 IFD6 RAC1 orf19.4749 orf19.1840 IRA2 orf19.4947 YPT52 FTR1 ATP18 orf19.1534 ZRT2 YPT72 GPA2 DTD2 CUP5 PRE3 ERG8 ARG8 GUT2 IFG3 orf19.4153 orf19.3983 VID27 FET34 OYE2 OYE23 orf19.3458 orf19.3475 orf19.5553 orf19.5597.1 AYR2 orf19.5614 orf19.1212 orf19.2124 orf19.1340 orf19.7502 RSR1 orf19.716 PHR1 PRA1 RVS167 HIS3 CTR1 VTC4 HAT2 orf19.6869 orf19.6868 HSP30 EMP24 orf19.1052 GAP4 GPX2 CMK2 RSP5 UBI3 CDC68 YVC1 GSH2 SUR7 orf19.3226 CPA2 PRN4 NDE1 YIM1 orf19.1723 HYR1 POB3 RPL8B;RPL82 CDR1;CDR2 ARF2;ARF1 TVP18 ATP6</t>
+          <t>orf19.6079 orf19.6066 orf19.4530.1 orf19.4476 IFD6 RAC1 orf19.5095 orf19.4749 orf19.1840 IRA2 orf19.4947 YPT52 FTR1 ATP18 orf19.1534 ZRT2 YPT72 GPA2 DTD2 CUP5 PRE3 ERG8 ARG8 GUT2 IFG3 orf19.4153 orf19.3983 VID27 FET34 OYE2 OYE23 orf19.3458 orf19.3475 orf19.5553 orf19.5597.1 AYR2 orf19.5614 orf19.1212 orf19.2124 orf19.1340 orf19.7502 RSR1 orf19.716 PHR1 PRA1 RVS167 HIS3 CTR1 VTC4 HAT2 orf19.6869 orf19.6868 HSP30 EMP24 orf19.1052 GAP4 GPX2 CMK2 RSP5 UBI3 CDC68 YVC1 GSH2 SUR7 orf19.3226 CPA2 PRN4 NDE1 YIM1 orf19.1723 HYR1 POB3 RPL8B;RPL82 CDR1;CDR2 ARF2;ARF1 TVP18 ATP6</t>
         </is>
       </c>
     </row>
@@ -1087,11 +1087,11 @@
         </is>
       </c>
       <c r="F10">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>GAL7 AGE3 orf19.2954 GLT1 NEP1 orf19.7244 ENT3 COX6 orf19.185 ECM17 orf19.2269 RNR22 APE3 GCN1 FOX2 ALI1 orf19.1682 orf19.1662 orf19.1626 orf19.7357 DNM1 orf19.7437 AAT22 SOD1 orf19.3810 OFD1 orf19.5698 orf19.1967 RPN8 orf19.3982 CIC1 TIF3 orf19.3480 orf19.3482 GCV1 orf19.5516 APA2 GBP2 orf19.6458.1 RPP1B orf19.7131 POT1 PCK1 LEU1 MRPL6 MLC1 RPS30 YDJ1 orf19.518 IFE2 RPP2A orf19.7288 PHO88 orf19.7322 orf19.6612 SIK1 orf19.7590 RPO21 MAL2 ATP16 PMT1 ADH2 COX1 orf19.2965 ERG11 orf19.1052;HTB1 orf19.1815 orf19.3755 orf19.51 ARO10 RPG1A orf19.397 SDH2 ICL1 NOP5 orf19.213 NDH51 ARO7 orf19.1162 EGD1 orf19.1862 LYS21 orf19.1030 GAL1 SKP1 EFG1 YWP1 orf19.2286 DQD1 orf19.2275 RNR1 NOP1 UBI3;UBI4 orf19.3430 orf19.969 MDH1-3 SCS7 orf19.512 orf19.498 MRPL40 SDS24 FUN12 RHR2 orf19.5420 orf19.3357 orf19.3349 ZPR1 HMT1 MGE1 orf19.6090 MRT4 orf19.5517 RFA1 orf19.4283 NUC2 TOM40 COQ6 orf19.3022 ARX1 TIF34 orf19.1709 orf19.1687 PUT2 HAS1 OSM2 CYB2 PRS1 orf19.1480 COX4 COX13 BGL2 BFR1 RPL8B ARF2 RPP2B URA1 RPP1A</t>
+          <t>GAL7 AGE3 orf19.2954 GLT1 orf19.7244 ENT3 COX6 orf19.185 ECM17 orf19.2269 RNR22 APE3 GCN1 FOX2 ALI1 orf19.1682 orf19.1626 orf19.7357 DNM1 orf19.7437 AAT22 SOD1 orf19.3810 OFD1 orf19.5698 RPN8 orf19.3982 CIC1 TIF3 orf19.3480 orf19.3482 GCV1 orf19.5516 APA2 GBP2 RPP1B POT1 PCK1 LEU1 MRPL6 MLC1 RPS30 YDJ1 orf19.518 IFE2 RPP2A orf19.7288 PHO88 orf19.7322 orf19.6612 SIK1 orf19.7590 RPO21 MAL2 ATP16 PMT1 ADH2 COX1 orf19.2965 ERG11 orf19.1052;HTB1 orf19.1815 orf19.3755 orf19.51 ARO10 RPG1A SDH2 ICL1 NOP5 orf19.213 NDH51 ARO7 orf19.1162 EGD1 orf19.1862 LYS21 orf19.1030 GAL1 SKP1 EFG1 YWP1 orf19.2286 DQD1 orf19.2275 RNR1 NOP1 UBI3;UBI4 orf19.3430 orf19.969 MDH1-3 SCS7 orf19.498 MRPL40 SDS24 FUN12 RHR2 orf19.5420 orf19.3357 orf19.3349 ZPR1 HMT1 MGE1 orf19.6090 MRT4 orf19.5517 RFA1 orf19.4283 NUC2 TOM40 COQ6 orf19.3022 ARX1 TIF34 orf19.1709 orf19.1687 PUT2 OSM2 CYB2 PRS1 orf19.1480 COX4 COX13 BGL2 BFR1 RPL8B ARF2 RPP2B URA1 RPP1A</t>
         </is>
       </c>
     </row>
@@ -1114,11 +1114,11 @@
         </is>
       </c>
       <c r="F11">
-        <v>306</v>
+        <v>231</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>RPO41 orf19.3325 MRP20 orf19.4532 orf19.3684 orf19.2930 PDE2 orf19.3027 orf19.3016 orf19.1037;IFI3 HMG1 orf19.5194.1 FMA1 PHO85 orf19.6843 orf19.6853 PRC3 orf19.6245 orf19.6211 ADE4 SMI1 UBA2 orf19.4735 SAC1 orf19.989 GCA2;GCA1 RPA190 orf19.2333 RPL82 orf19.2330 orf19.2305 orf19.670.2 CTA3 orf19.5239 CDC54 orf19.4952.1 KEM1 orf19.7234 orf19.2111 orf19.2095 orf19.2019 RAD23 orf19.1516 orf19.1578 HYU1 ADE8 TOM1 HEM2 NSP1 GCD7 RIM11;orf19.792 orf19.4504 orf19.4492 RPC40 orf19.3559 TPK2 orf19.2278 MCM3 orf19.2214 TIF4631 GLO2 CDC47 orf19.1389 orf19.200 MET10 SGT1 orf19.1381 YOR1 MRPL33 orf19.1697 UTP4 AIP2 ALT1 orf19.6966 orf19.7368 orf19.7404 orf19.6787 orf19.6189 orf19.6718 orf19.5665 PWP1 orf19.2686 MSN5 orf19.2664 orf19.5038 RRP42 orf19.3792 ALD6 orf19.1791 orf19.1272 AGO1 orf19.3124 AFL1 orf19.581 orf19.577 orf19.1956 orf19.1961 orf19.1940 SNF1 MAS2 orf19.3185 orf19.4225.1 orf19.4316 orf19.6665 orf19.2639.1 GUK1 orf19.3957 orf19.4030 RPN5 orf19.4193 orf19.92 DOG1 orf19.3499 orf19.5730 orf19.5747 SNF4 orf19.73 orf19.1086 orf19.1085 VPS70 orf19.7097 RPA135 orf19.7067 ACB1 orf19.7011 YML6 orf19.7012 GCN3 orf19.5131 orf19.5161 orf19.1335 orf19.7200 MRP7 NPT1 KAP120 UTP18 orf19.7499 orf19.7485 NTH1 orf19.2520 PAN6 orf19.2835 ACO2 orf19.3704.1 TPM2 PDK2 orf19.7290 ELF1 YKE2 orf19.6602 MSS51 CTM1 orf19.5158 PHR2 CHS5 MRPS9 orf19.6676;orf19.1124.2 DUT1 CDC21 HIS1 CGR1 SPL1 SPT6 SIT4 ESS1 MYO5 CTN3 orf19.1857 RPB8 HAM1 GLY1 orf19.4204 orf19.6346 GCF1 orf19.399 orf19.394 CAF16 orf19.6693 MRPL8 orf19.3477 SPS20 CTN1 PPZ1 orf19.5666 RAD51 GPM2 HTA2 ERB1 SMT3 YPD1 orf19.2352 UBA4 orf19.2306 ARC18 orf19.109 orf19.4107 PES1 orf19.585 HAL22 orf19.3585 SSO2 GIS2 RFA2 MRPL10 CKA2 TIF35 orf19.7215 orf19.4382 orf19.4375 MCM2 orf19.7153 SER2 orf19.5812 orf19.3136 orf19.2920 orf19.439 orf19.7459 ECI1 orf19.6424 orf19.5250 orf19.5235 orf19.5229 orf19.1248 BDF1 orf19.967 VPS2 NAM7 orf19.5168 orf19.5321 orf19.5293 LYS4 MRP8 orf19.3836 orf19.3797 orf19.500 DRG1 MRPL3 GLO3 CAB3 SKI8 orf19.5757 ISN1 orf19.3312 orf19.2518 ARP9 orf19.2484 orf19.2438 NAP1 MRPL19 KEL1 NAA25 orf19.5522 ARP4 HCR1 orf19.6822 orf19.6804 SSN6 YSA1 HHT1;HHT2;HHT21 MET8 GCD2 orf19.6752 orf19.6748 orf19.6739 orf19.6717 orf19.345 MET13 KEX1 orf19.4306 orf19.6585 orf19.6554 orf19.6503 orf19.904 orf19.863 GNA1 SDS22 ACP12 orf19.3045 SEC62 COQ4 TOM20 FOX3 CDC53 ILV3 orf19.4021 orf19.4018 orf19.3977 SSD1 DOS2 GCV3 orf19.4960 orf19.4932 orf19.1565 orf19.4611 TYR1 orf19.4597 CLC1 orf19.5965 orf19.5885 orf19.4894 orf19.4850 YTM1 orf19.4796 orf19.4751 HBR1 THR1</t>
+          <t>orf19.3325 orf19.4532 orf19.3684 orf19.2930 PDE2 orf19.3016 orf19.1037;IFI3 HMG1 orf19.5194.1 FMA1 PHO85 orf19.6853 PRC3 ADE4 SMI1 orf19.4735 SAC1 orf19.989 GCA2;GCA1 RPA190 orf19.2333 RPL82 orf19.670.2 CTA3 KEM1 orf19.7234 orf19.2095 orf19.1578 ADE8 TOM1 HEM2 NSP1 GCD7 RIM11;orf19.792 orf19.4504 RPC40 orf19.3559 TPK2 orf19.2278 MCM3 orf19.2214 TIF4631 GLO2 orf19.1389 orf19.200 MET10 SGT1 orf19.1381 YOR1 MRPL33 orf19.1697 AIP2 ALT1 orf19.7368 orf19.7404 orf19.6787 orf19.6189 orf19.6718 orf19.5665 orf19.2686 orf19.5038 RRP42 orf19.3792 ALD6 orf19.1272 AGO1 orf19.3124 AFL1 orf19.581 orf19.577 orf19.1956 orf19.1961 SNF1 orf19.3185 orf19.4225.1 orf19.4316 orf19.6665 GUK1 RPN5 orf19.4193 orf19.92 DOG1 orf19.5730 orf19.5747 SNF4 orf19.73 orf19.1086 orf19.1085 orf19.7097 RPA135 orf19.7067 ACB1 orf19.7011 YML6 orf19.7012 GCN3 orf19.5161 orf19.7200 MRP7 NPT1 KAP120 orf19.7499 orf19.7485 NTH1 orf19.2520 PAN6 orf19.2835 ACO2 orf19.3704.1 TPM2 orf19.7290 YKE2 orf19.6602 MSS51 orf19.5158 PHR2 MRPS9 orf19.6676;orf19.1124.2 DUT1 CDC21 HIS1 SPL1 SIT4 MYO5 CTN3 RPB8 HAM1 orf19.4204 orf19.6346 GCF1 orf19.394 CAF16 orf19.6693 MRPL8 PPZ1 RAD51 GPM2 HTA2 SMT3 YPD1 orf19.2352 UBA4 orf19.2306 ARC18 orf19.109 orf19.4107 PES1 orf19.585 HAL22 orf19.3585 SSO2 RFA2 MRPL10 CKA2 TIF35 orf19.7215 orf19.4382 MCM2 orf19.7153 SER2 orf19.5812 orf19.2920 orf19.439 orf19.6424 orf19.5235 orf19.5229 orf19.1248 BDF1 orf19.967 orf19.5321 orf19.5293 LYS4 MRP8 orf19.3797 DRG1 MRPL3 GLO3 CAB3 ISN1 orf19.3312 orf19.2518 ARP9 orf19.2484 orf19.2438 NAP1 MRPL19 NAA25 ARP4 HCR1 orf19.6822 orf19.6804 HHT1;HHT2;HHT21 GCD2 orf19.6752 orf19.6748 orf19.6739 orf19.6717 orf19.345 MET13 KEX1 orf19.4306 orf19.6554 orf19.6503 orf19.904 orf19.863 SDS22 ACP12 orf19.3045 SEC62 TOM20 FOX3 CDC53 ILV3 orf19.4018 orf19.3977 SSD1 DOS2 GCV3 orf19.4960 orf19.4932 orf19.1565 TYR1 orf19.4597 orf19.5885 orf19.4894 orf19.4850 YTM1 orf19.4796 orf19.4751 HBR1 THR1</t>
         </is>
       </c>
     </row>
@@ -1168,11 +1168,11 @@
         </is>
       </c>
       <c r="F13">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>MAS1 NPL3 RPC10 orf19.3528 orf19.2259 orf19.158 PPT1 PTC7 orf19.1953 orf19.1180 orf19.2143 orf19.7478 orf19.639.1 BET2 CKS1 orf19.2639 NMD5 orf19.2426 PRS5 orf19.5279 orf19.7291 DED1 orf19.3446 LEU4 orf19.5611 SOD5 orf19.1545</t>
+          <t>MAS1 orf19.2305 NPL3 RPC10 orf19.3528 orf19.2259 orf19.158 PPT1 orf19.1953 orf19.1180 orf19.3499 orf19.7478 orf19.639.1 BET2 CTM1 CKS1 orf19.2639 CTN1 GIS2 orf19.2426 PRS5 orf19.5279 DED1 orf19.3446 VPS2 LEU4 orf19.5611 SOD5 COQ4 CLC1</t>
         </is>
       </c>
     </row>
@@ -1195,11 +1195,11 @@
         </is>
       </c>
       <c r="F14">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>SSH1 orf19.4758 orf19.2257 orf19.5660.1 orf19.2917 ASR2 ERG5 ATP20 NOC2 HEM15 orf19.4396 PMT2 EMP70</t>
+          <t>SSH1 orf19.4758 NEP1 orf19.2257 orf19.1662 orf19.5660.1 orf19.2917 orf19.1967 orf19.6458.1 orf19.7131 ASR2 ERG5 ATP20 NOC2 orf19.397 HEM15 orf19.4396 orf19.512 PMT2 EMP70 HAS1</t>
         </is>
       </c>
     </row>
@@ -1222,11 +1222,11 @@
         </is>
       </c>
       <c r="F15">
-        <v>99</v>
+        <v>164</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>SIN3 orf19.3333 orf19.6259 orf19.4437;ISW2 GCS1 GCR3 orf19.4888 orf19.4901 DJP1 orf19.2328 ERP5 CHS3 HGT7 UTP22 orf19.5834 orf19.5783 orf19.880 orf19.4488 orf19.3547 orf19.3552 orf19.3556 orf19.2228 orf19.2265 PUS7 UTP20 GEA2 OST1 YCK2 NOG1 STE24 MLP1 UBR1 orf19.3183 orf19.4228 DAP2 RMS1 MTR10 orf19.4029 FCA1 HOC1 NIP7 orf19.5541 POL5 orf19.7116 orf19.7041 PHM5 orf19.2371 POL3 orf19.2372 LMO1 orf19.1338 orf19.7197 orf19.7160 ATP17 MCM6 orf19.2820 DOM34 RGD3;orf19.730 URA3 CDC28 MNN9 orf19.6284 SDA1 NMD3 RTS1 orf19.6838 orf19.4164 orf19.4537 RPL7 orf19.1782 UTP15 RPF2 PLC2;FGR22 TSR1 orf19.3798 orf19.477 OLE1 PBP2 orf19.5763 SEC65 NPL4 DRS1 MSF1 orf19.2017 orf19.6783 orf19.320 RVS161 orf19.4340 VPS4 orf19.3947 SPT5 orf19.1449 orf19.1495 TOA2 SEC7 PKC1 orf19.4846 MSS116 GDA1</t>
+          <t>RPO41 SIN3 orf19.3333 MRP20 orf19.3027 orf19.6843 orf19.6245 orf19.6259 orf19.6211 orf19.4437;ISW2 GCS1 UBA2 GCR3 orf19.4888 orf19.4901 DJP1 orf19.2328 orf19.2330 ERP5 orf19.5239 CDC54 CHS3 orf19.4952.1 orf19.2111 HGT7 orf19.2019 RAD23 orf19.1516 UTP22 orf19.5834 HYU1 orf19.5783 orf19.880 orf19.4492 orf19.4488 orf19.3547 orf19.3552 orf19.3556 orf19.2228 orf19.2265 CDC47 PUS7 UTP20 GEA2 UTP4 orf19.6966 OST1 YCK2 NOG1 STE24 MLP1 PWP1 UBR1 MSN5 orf19.2664 orf19.1791 orf19.1940 MAS2 orf19.3183 orf19.4228 DAP2 RMS1 orf19.2639.1 MTR10 orf19.3957 orf19.4030 orf19.4029 FCA1 HOC1 NIP7 orf19.5541 POL5 orf19.7116 VPS70 orf19.7041 PHM5 orf19.2371 POL3 orf19.2372 orf19.5131 LMO1 orf19.1338 orf19.1335 orf19.7197 orf19.7160 UTP18 MCM6 orf19.2820 DOM34 RGD3;orf19.730 PDK2 ELF1 CHS5 URA3 CDC28 MNN9 CGR1 SPT6 ESS1 orf19.1857 orf19.6284 GLY1 SDA1 NMD3 RTS1 orf19.399 orf19.6838 orf19.3477 orf19.4164 SPS20 orf19.4537 orf19.5666 RPL7 ERB1 orf19.1782 UTP15 RPF2 orf19.4375 PLC2;FGR22 orf19.3136 orf19.7459 ECI1 TSR1 orf19.5250 NAM7 orf19.5168 orf19.3836 orf19.3798 orf19.500 orf19.477 OLE1 PBP2 SKI8 orf19.5763 orf19.5757 SEC65 KEL1 orf19.5522 DRS1 MSF1 orf19.2017 SSN6 YSA1 orf19.6783 MET8 orf19.320 RVS161 orf19.4340 VPS4 orf19.6585 GNA1 orf19.4021 orf19.3947 SPT5 orf19.1449 orf19.1495 TOA2 orf19.4611 orf19.5965 SEC7 PKC1 orf19.4846 MSS116 GDA1</t>
         </is>
       </c>
     </row>
@@ -1326,11 +1326,11 @@
         </is>
       </c>
       <c r="F2">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>orf19.6066 HGT1 RAC1 ERO1 CHS3 PLB4.5 MSB2 RHO3 PHM7 YCK2 orf19.6741 FET34 YPT31 PHR2 CDC42 PHR1 PGA52 SAP9 GAP4 MP65 SSO2 YVC1 SUR7 ENA21 CRH11 YKT6 PGA4 CDR1;CDR2 GSC1 ECM33 orf19.1054 PMA1 orf19.3799 FAA4 RHO1 POR1 MNT1 VAC8 YWP1 HGT6 BGL2 MIR1 MTS1</t>
+          <t>HGT1 RAC1 ERO1 CHS3 HGT7 PLB4.5 MSB2 RHO3 PHM7 YCK2 orf19.6741 FET34 PHR2 CDC42 PHR1 PGA52 SAP9 GAP4 MP65 SUR7 ENA21 CRH11 YKT6 PGA4 CDR1;CDR2 GSC1 ECM33 orf19.1054 orf19.2168.3 PMA1 orf19.3799 RHO1 POR1 VAC8 YWP1 HGT6 BGL2 MIR1 MTS1</t>
         </is>
       </c>
     </row>
@@ -1353,11 +1353,11 @@
         </is>
       </c>
       <c r="F3">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>KEX2 orf19.4805 YPT52 TOS1 SCW11 CHS2 PLB3 MNT2 ALS3 RBT1 RSP5 ENG1 HYR1 orf19.3341 orf19.2489 HET1 SEC4 TIF NOP5 orf19.1355 GUA1</t>
+          <t>orf19.4805 TOS1 SCW11 CHS2 PLB3 MNT2 ALS3 RBT1 RSP5 ENG1 HYR1 orf19.3341 orf19.2489 HET1 SEC4 TIF orf19.86</t>
         </is>
       </c>
     </row>
@@ -1380,11 +1380,11 @@
         </is>
       </c>
       <c r="F4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>HGT7 ARF3 VPH1 YPT1 orf19.6264.3 orf19.2168.3 ACC1 EMP70</t>
+          <t>ARF3 VPH1 YVC1 YPT1 orf19.6264.3 MNT1 EMP70</t>
         </is>
       </c>
     </row>
@@ -1407,11 +1407,11 @@
         </is>
       </c>
       <c r="F5">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>PLB5 orf19.1152 orf19.5006.1 RSR1 AHA1 CHT2 SAP5 orf19.3335 YPS7 NCE102 GDI1 VAS1 SAC6 VMA13 URA2 orf19.86 RAS1 orf19.1946 FAS1 TPD3</t>
+          <t>PLB5 orf19.5006.1 YPT52 RSR1 AHA1 CHT2 SAP5 orf19.3335 YPS7 NCE102 VMA13 SOD5</t>
         </is>
       </c>
     </row>
@@ -1434,11 +1434,11 @@
         </is>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>VTC4 COI1 VTC3</t>
+          <t>orf19.6066 VTC4 SSO2 COI1 VTC3 FAA4</t>
         </is>
       </c>
     </row>
@@ -1461,11 +1461,11 @@
         </is>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>SUB2 BUD7</t>
+          <t>KEX2 VMA6 NOP5 orf19.1355 GUA1</t>
         </is>
       </c>
     </row>
@@ -1488,11 +1488,11 @@
         </is>
       </c>
       <c r="F8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>PEP1 FMP45 YCF1 YCP4 ADP1 SLP3 orf19.2163</t>
+          <t>PEP1 FMP45 YCF1 YCP4 ADP1 YPT31 SLP3 orf19.2163 ACC1</t>
         </is>
       </c>
     </row>
@@ -1515,11 +1515,11 @@
         </is>
       </c>
       <c r="F9">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>PLD1 NCR1 orf19.1448.1 orf19.1766 orf19.374 CFL2 ZRT1 ALS4 orf19.7056 XOG1 ECE1 CTR1 SUN41 FRE10 VCX1 SIT1 BMT3 CRL1 PBR1 orf19.6077 ASM3 SAP6 orf19.7578 SMF3 SOD5 DCW1 DPP3 EXG2 SIM1 orf19.4780 orf19.6079 RPN1 FTR1 orf19.7214 orf19.1534 ZRT2 YPT72 TPS3 GPA2 RPL18 VMA6 GLC3 GUS1 GPH1 UBC4 CEF3 HXK2 GSP1 HSP30 EFT2 UBI3 SEC23 SRV2 GSY1 RDI1 ARF2;ARF1 orf19.4898 TVP18 SEC24 TPS1 RPL10A</t>
+          <t>PLD1 NCR1 orf19.1448.1 orf19.1766 orf19.374 CFL2 ZRT1 ALS4 orf19.7056 XOG1 ECE1 CTR1 SUN41 FRE10 VCX1 SIT1 BMT3 CRL1 PBR1 orf19.6077 ASM3 SAP6 orf19.7578 SMF3 DCW1 DPP3 EXG2 SIM1 orf19.4780 orf19.6079 orf19.1152 RPN1 FTR1 orf19.7214 GDI1 orf19.1534 ZRT2 VAS1 YPT72 TPS3 GPA2 RPL18 SUB2 SAC6 GLC3 GUS1 GPH1 URA2 UBC4 CEF3 HXK2 BUD7 GSP1 HSP30 RAS1 EFT2 UBI3 orf19.1946 SEC23 FAS1 SRV2 GSY1 TPD3 RDI1 ARF2;ARF1 orf19.4898 TVP18 SEC24 TPS1 RPL10A</t>
         </is>
       </c>
     </row>
@@ -1542,11 +1542,11 @@
         </is>
       </c>
       <c r="F10">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>orf19.6082 orf19.2460 WBP1 CTP1 OST1 ERG251 GUT2 orf19.4131 orf19.3983 YHM1 SNQ2 SEC63 orf19.3518 orf19.6119 YHM2 SPF1 KTR4 GNP1 PTR22 orf19.6887 HGT2 GPD2 YMC1 ALP1 FAD2 GPX2 orf19.3558 SUR2 orf19.1239 OLE1 IFF11 ERG27 PGA45 CHT1 NUO2 YIM1 orf19.1691 orf19.3994 STT3 orf19.4706 GDA1 ERG1 NAD5 ATP6 KAR2 QCR8 orf19.1682 PHB1;orf19.357 RIP1 orf19.4016 NUO1 ALO1 ERG11 GFA1 QCR2 TOM70 TIM50 PET9 MLT1 RHR2 orf19.6035 COX5 COX2</t>
+          <t>orf19.6082 orf19.2460 WBP1 OST1 ERG251 GUT2 YHM1 SNQ2 SEC63 orf19.6119 SPF1 KTR4 GNP1 PTR22 orf19.6887 GPD2 YMC1 ALP1 FAD2 orf19.3558 SUR2 orf19.1239 OLE1 IFF11 ERG27 PGA45 CHT1 NUO2 YIM1 orf19.4706 GDA1 ERG1 PHB1;orf19.357 orf19.4016 NUO1 ALO1 GFA1 TOM70 TIM50 PET9 MLT1 orf19.6035</t>
         </is>
       </c>
     </row>
@@ -1569,11 +1569,11 @@
         </is>
       </c>
       <c r="F11">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>DIP5 orf19.2439.1 CDR4 SAM4 GCR3 GAR1 orf19.5274 SPA2 OP4 ATP18 orf19.1533 orf19.1549 FRP3 ERG9 FLO9 orf19.1655.3 APL2 CHS4 orf19.2757 orf19.4153 orf19.1179 PLB2 orf19.1212 orf19.2124 GYP7 orf19.7198 FLC2 EMP46 ERG5 SAP3 CHT3 DBP2 MNN26 orf19.5669 ERG3 PHO100 MNN2 orf19.2246 CDC68 AQY1 RHD3 LAG1 MNN24 SLC1 SAP8 orf19.6565 UTR2 RAT1 HGH1 PKC1 DBP3 SSU81 PLB1 orf19.2954 ATP1 HPT1 LHS1 orf19.6883 orf19.5682 CDC60 SIK1 orf19.1833 HSP90 ILS1 orf19.7153 KRE30 SER33 TOM40 APT1 NIP1</t>
+          <t>DIP5 CDR4 SAM4 ATP18 orf19.1533 FRP3 ERG9 FLO9 orf19.1655.3 CHS4 orf19.2757 orf19.4153 orf19.1179 orf19.1212 orf19.7198 FLC2 CHT3 DBP2 MNN26 orf19.5669 ERG3 orf19.2246 LAG1 MNN24 SLC1 SAP8 UTR2 HGH1 DBP3 SSU81 PLB1 GCR3 HPT1 orf19.6883 CRM1 ERG5 APT1 NIP1</t>
         </is>
       </c>
     </row>
@@ -1596,11 +1596,11 @@
         </is>
       </c>
       <c r="F12">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>IST2 SAC1 orf19.2328 ERP5 NOG1 STE24 ATP17 orf19.7307 ERV25 orf19.2017 orf19.3060 SSH1 CYT1 orf19.2257 ADH2 ATP20 ATP7 orf19.3859 ATP4 UBI3;UBI4 PMT2 SEC61</t>
+          <t>orf19.2328 ERP5 STE24 orf19.4131 ATP17 orf19.3518 orf19.7307 GPX2 ERV25 orf19.3060 SSH1 KAR2 orf19.2257 RIP1 COX1 QCR2 ATP20 NDH51 orf19.3859 PMT2 COX2</t>
         </is>
       </c>
     </row>
@@ -1623,11 +1623,11 @@
         </is>
       </c>
       <c r="F13">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>SNO1 orf19.4758 CRP1 orf19.4955 MUQ1 orf19.5783 orf19.4127 orf19.1785 PUS7 orf19.5660.1 orf19.4228 HEX1 SFC1 HOC1 orf19.6553 LMO1 APL4 FLU1;TPO2 SAP2 CDC28 RVS167 orf19.6284 HEM15 EMP24 orf19.1782 MNN22 ALS1 NPL4 orf19.6200 orf19.2059 DFI1 SSR1 MNN1 ECM331 MAL31 SPT5 PHO114 MNN12 LIP4 TUB2 GGA2 SEC21 orf19.1229 RPL14 ASN1 FAS2 CAM1 IDI1 TRP5 THS1 CAM1-1 CHC1 CRM1 IFR2 RPS3 CBP1 SEC14 orf19.51 RPG1A orf19.3681 TAL1 GLO3 RPS21 orf19.4248 ARF2 TPI1</t>
+          <t>SNO1 orf19.4758 CRP1 OP4 orf19.4955 orf19.5783 orf19.4127 orf19.1785 APL2 orf19.5660.1 orf19.4228 HEX1 SFC1 HOC1 PLB2 orf19.2124 orf19.6553 LMO1 GYP7 APL4 FLU1;TPO2 SAP3 SAP2 RVS167 EMP24 PHO100 MNN2 orf19.1782 CDC68 RHD3 MNN22 ALS1 NPL4 orf19.6200 orf19.2059 DFI1 SSR1 MNN1 ECM331 MAL31 PHO114 PKC1 MNN12 LIP4 RPL14 LHS1 CAM1 IDI1 TRP5 CAM1-1 CHC1 IFR2 TAL1 TOM40 ARF2</t>
         </is>
       </c>
     </row>
@@ -1650,11 +1650,11 @@
         </is>
       </c>
       <c r="F14">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>HMG1 PHO84 orf19.2091 orf19.6828.1 SEC8 orf19.7672 VPS21 orf19.2821 DED1 PMT6 orf19.5077 BNA4 NDE1 orf19.5991 MAK21 ALI1 GDH3 orf19.5547 ERG6 NUC2 ERV29</t>
+          <t>PHO84 orf19.2091 orf19.1578 CTP1 NOG1 orf19.6828.1 orf19.3983 SEC8 orf19.7011 orf19.7672 YHM2 HGT2 VPS21 orf19.2821 DED1 PMT6 orf19.5077 BNA4 NDE1 orf19.1691 orf19.3994 MYO2 STT3 orf19.5991 MAK21 NAD5 ATP6 QCR8 CYT1 orf19.5547 PHO88 ERG11 RHR2 ERV29 COX5 SEC61</t>
         </is>
       </c>
     </row>
@@ -1677,11 +1677,11 @@
         </is>
       </c>
       <c r="F15">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>RPO41 orf19.3293 orf19.3304 ROA1 orf19.2964 MAS1 EHT1 NOP4 orf19.2485 PHO87 orf19.5095 orf19.1139 CSI2 orf19.6355 NPL3 RPC10 DDI1 UTP21 orf19.804.1 orf19.3583 orf19.2165 SLP2 FCY21 orf19.1404 CHS8 orf19.158 PPT1 KRE5 KRE6 PBS2 orf19.6828 NUP159 PTC7 orf19.4686 orf19.3367 orf19.3782.2 orf19.3141 orf19.3128 orf19.3914 orf19.688 NAB3 orf19.5607 NOG2 NUP82 CDC39 orf19.2143 orf19.7069 orf19.7088 PEL1 NOP15 ENP1 orf19.7478 orf19.501 orf19.639.1 orf19.7326 ELF1 orf19.6597 BET2 RFC4 HEM3 COB NSA2;orf19.7397.1;orf19.7397.1;orf19.7398 MEX67 IPK1 orf19.5206 orf19.1849 orf19.409 orf19.4479 DBP7 orf19.3463 NMD5 CCC1 orf19.6868 orf19.1305 orf19.1304 IMP4 TIM23 AAH1 orf19.4373 orf19.1970 orf19.2426 PRS5 orf19.7291 orf19.3446 orf19.5356 orf19.547 TIM44 orf19.5442 HGT10 PRN4 CNS1 orf19.5515 orf19.7546 NDT80 UTP9 GIR2 EXO70 ARX1 orf19.1646 orf19.1545 orf19.5989 SFH5 AGE3 RPL6 FMA1 YBN5 ADE5,7 orf19.5085 orf19.1514 orf19.6787 ATP2 orf19.1409.1 orf19.5627 GLN4 FRS1 NMT1 SSA2 IMH3 DED81 orf19.6701 SAR1 CYS4 ERF1 SER2 NOP1 KRS1 orf19.3037</t>
+          <t>orf19.3293 orf19.3304 ROA1 orf19.2964 EHT1 NOP4 orf19.2485 orf19.2439.1 PHO87 orf19.5095 GAR1 orf19.1139 orf19.5274 CSI2 orf19.6355 SPA2 NPL3 RPC10 DDI1 orf19.1549 UTP21 orf19.804.1 orf19.3583 orf19.2165 SLP2 FCY21 orf19.1404 CHS8 orf19.158 PPT1 KRE5 KRE6 PBS2 orf19.6828 NUP159 PTC7 orf19.4686 orf19.3367 orf19.3782.2 orf19.3141 orf19.3128 orf19.3914 orf19.688 NAB3 orf19.5607 NOG2 NUP82 CDC39 orf19.2143 orf19.7069 orf19.7088 PEL1 NOP15 ENP1 orf19.7478 orf19.501 orf19.639.1 EMP46 orf19.7326 orf19.6597 BET2 RFC4 HEM3 COB NSA2;orf19.7397.1;orf19.7397.1;orf19.7398 MEX67 IPK1 orf19.5206 orf19.1849 orf19.409 orf19.4479 DBP7 orf19.3463 NMD5 CCC1 orf19.6868 orf19.1305 orf19.1304 IMP4 TIM23 AAH1 orf19.4373 orf19.1970 orf19.2426 AQY1 orf19.7291 orf19.5356 orf19.547 TIM44 orf19.5442 HGT10 PRN4 CNS1 orf19.5515 orf19.7546 NDT80 UTP9 GIR2 orf19.6565 EXO70 orf19.1646 orf19.1545 RAT1 orf19.5989 SFH5 RPL6 YBN5 ADE5,7 orf19.1229 orf19.5085 orf19.3810 orf19.5682 orf19.5627 GLN4 CDC60 FRS1 ELF1 SIK1 orf19.1833 orf19.2965 NMT1 HSP90 SUI1 DED81 orf19.6701 CYS4 orf19.1030 ERF1 orf19.7153 SER2 NOP1 KRE30 SER33 orf19.3045 orf19.3037 THR1</t>
         </is>
       </c>
     </row>
@@ -1704,11 +1704,11 @@
         </is>
       </c>
       <c r="F16">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>orf19.3290 MRS7 orf19.2988 orf19.4468 orf19.6233 PEX3 orf19.5079.1 orf19.1840 FTR1;FTR2 HMA1 orf19.2002 ZRC1 orf19.1578 TOM1 orf19.875 TIF4631 TIM22 orf19.216.1 orf19.4066 ERG4 SCT1 orf19.6951 SAM50 orf19.7386 orf19.3366.1 orf19.5300 YME1 SAM51 orf19.1956 orf19.3920 SRP101 orf19.5628 orf19.1086 orf19.7011 orf19.6898.1 HLJ1 orf19.4380.1 orf19.6318 orf19.641 orf19.697 orf19.7304 SCO1 MSS51 PTP3 MNN9 orf19.556 URA6 ALG2 FAT1 orf19.6627 NMD3 PAM18 SPC2 RIM2 CWH8 PHO91 PMT4 orf19.3611 MAK5 ERG26 VMA5 orf19.7459 orf19.6438 orf19.6396 MCD4 orf19.5296 CRC1 orf19.2484 HMX1 orf19.6062 PSD1 DRS1 PMT5 DFG5 orf19.2057 ERG28 PAM17 SSD1 LCB2 MYO2 AGC1 orf19.1546 orf19.6007 MSS116 NAD4 SEC18 orf19.1564 COX6 COX9 FAA21 VPS1 SUI3 ATP3 TUB1 PHO88 orf19.7590 PMT1 COX1 SAH1 LSP1 CBR1 SDH2 NDH51 orf19.2335 GPD1 orf19.4396 SDH12 orf19.6435 SCS7 QCR7 FESUR1 DBP5 HAS1 orf19.1480 COX4 COX13 URA1</t>
+          <t>orf19.3290 MRS7 orf19.2988 HMG1 orf19.4468 orf19.6233 PEX3 IST2 orf19.5079.1 SAC1 orf19.1840 FTR1;FTR2 HMA1 orf19.2002 ZRC1 TOM1 orf19.875 TIF4631 TIM22 orf19.216.1 orf19.4066 ERG4 SCT1 orf19.6951 SAM50 orf19.7386 orf19.3366.1 orf19.5300 YME1 SAM51 orf19.1956 orf19.3920 SRP101 orf19.5628 orf19.1086 orf19.6898.1 HLJ1 orf19.4380.1 orf19.6318 orf19.641 orf19.697 orf19.7304 SCO1 MSS51 PTP3 MNN9 orf19.556 URA6 ALG2 FAT1 orf19.6627 NMD3 PAM18 SPC2 RIM2 CWH8 PHO91 PMT4 orf19.3611 MAK5 ERG26 VMA5 orf19.7459 orf19.6438 orf19.6396 MCD4 orf19.5296 CRC1 orf19.2484 HMX1 orf19.6062 PSD1 DRS1 PMT5 DFG5 orf19.2057 orf19.2017 ERG28 PAM17 SSD1 LCB2 AGC1 orf19.1546 orf19.6007 MSS116 NAD4 SEC18 orf19.1564 COX6 COX9 ALI1 orf19.1682 FAA21 GDH3 VPS1 SUI3 ATP3 TUB1 orf19.7590 PMT1 ERG6 ADH2 SAH1 LSP1 CBR1 ATP7 SDH2 orf19.2335 GPD1 ATP4 orf19.4396 UBI3;UBI4 SDH12 orf19.6435 SCS7 QCR7 FESUR1 NUC2 DBP5 HAS1 orf19.1480 COX4 COX13 URA1</t>
         </is>
       </c>
     </row>
@@ -1781,11 +1781,11 @@
         </is>
       </c>
       <c r="F2">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>orf19.3053 orf19.449 GCV2 orf19.7215.3 orf19.7263 IDP1 orf19.1889 ETR1 SCL1 LAP41 orf19.5943.1 orf19.2755 XKS1 NIF3 OYE32 STI1 orf19.4230 orf19.5620 orf19.2125 PDX3 KGD2 orf19.6596 GRP2 orf19.1433 GDB1 GLR1 PUP2 LPD1 MET15 orf19.590 URA4 TIF11 DOT5 TMA19 SOD2 GCY1 GLX3 AMS1 ABP1 orf19.2966 HOM2 orf19.5961 SBP1 NHP6A IDH1 ILV5 GPM1 IPP1 PGI1 MCR1 APR1 YNK1</t>
+          <t>orf19.449 GCV2 orf19.7215.3 orf19.7263 IDP1 ETR1 SCL1 orf19.5943.1 XKS1 NIF3 OYE32 STI1 orf19.4230 orf19.5620 orf19.2125 orf19.6596 orf19.1433 GDB1 GLR1 LPD1 MET15 orf19.590 URA4 TIF11 DOT5 TMA19 SOD2 GCY1 GLX3 AMS1 orf19.2966 HOM2 SBP1 NHP6A IDH1 HSP60 GPM1 PGI1 APR1 YNK1</t>
         </is>
       </c>
     </row>
@@ -1808,11 +1808,11 @@
         </is>
       </c>
       <c r="F3">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>orf19.3689 LPG20 orf19.2794 GRE2 orf19.1860.1 orf19.4639 HSP12;orf19.4216 PRE8 PUP1 UGA2 NIT3 PRE2 SGT2 orf19.6423 OFR1 RIM1 TTR1 orf19.2036 orf19.6809 PRE1 CDC55 ADH5</t>
+          <t>orf19.3689 LPG20 orf19.2794 GRE2 orf19.1860.1 orf19.4639 HSP12;orf19.4216 PRE8 PUP1 UGA2 NIT3 PRE2 SGT2 OFR1 RIM1 TTR1 orf19.2036 orf19.6809 PRE1 CDC55</t>
         </is>
       </c>
     </row>
@@ -1835,11 +1835,11 @@
         </is>
       </c>
       <c r="F4">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>RIB4 TRP99 LHP1 TRP3 BAT22 ILV6 TIF5 orf19.2150 MAM33 orf19.7522 ARC40 orf19.1214 SER1 ILV1 MBF1 LYS12 PRO2 RVB2 HTS1 CPR3 CAT2 EGD2 EFB1 THR4 SHM1 LSC2 HSP60 PDA1 MDH1-1</t>
+          <t>orf19.3053 TRP99 LHP1 TRP3 orf19.1889 ILV6 orf19.2755 orf19.2150 MAM33 orf19.7522 PDX3 ARC40 SER1 ILV1 MBF1 LYS12 ABP1 HTS1 CPR3 CAT2 EGD2 EFB1 SHM1</t>
         </is>
       </c>
     </row>
@@ -1862,11 +1862,11 @@
         </is>
       </c>
       <c r="F5">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>orf19.7264 BAT21 CIP1 HCH1 orf19.7108 orf19.7152 PTC2 SHP1 orf19.715 ARC15 ARG3 orf19.2008 RKI1 CDC37 RPS21B ILV2 RPS19A orf19.6507 YRB1 RPN10 PR26 RPS20 CCT8 CPR6 GRX3 orf19.3037 HOM6 ADE2 SES1</t>
+          <t>orf19.7264 CIP1 HCH1 orf19.7108 orf19.7152 PTC2 SHP1 orf19.715 ARC15 ARG3 RKI1 CDC37 YRB1 orf19.3037 SES1</t>
         </is>
       </c>
     </row>
@@ -1889,11 +1889,11 @@
         </is>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>GAL10 PNP1 SOD3 PRE5 PHHB KGD1 ACH1 MDH1 MRF1 AHP1</t>
+          <t>GAL10 AAT1 LAP41 PNP1 BAT22 SOD3 PRE5 KGD2 GRP2 PHHB orf19.5961 ILV5 ACH1 MDH1 MRF1 orf19.2244 AHP1</t>
         </is>
       </c>
     </row>
@@ -1916,7 +1916,12 @@
         </is>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>orf19.6423 ADH5</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -1938,11 +1943,11 @@
         </is>
       </c>
       <c r="F8">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>TAF14 AAT1 orf19.5689 orf19.5525 ADO1 RPS28B orf19.5184 TYS1 SSC1 orf19.2244 MET14</t>
+          <t>RIB4 TAF14 orf19.5689 TIF5 orf19.5525 ADO1 RPS28B orf19.5184 orf19.1214 PUP2 PRO2 TYS1 RVB2 KGD1 THR4 LSC2 IPP1 SSC1 MCR1 PDA1 MET14 MDH1-1</t>
         </is>
       </c>
     </row>
@@ -1965,11 +1970,11 @@
         </is>
       </c>
       <c r="F9">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>orf19.71 ARG5,6 ERG12 RBK1 MUQ1 RPL38 DCK1 orf19.6867 orf19.3572.3 DTD2 PRE3 HIS5 ERG8 ARG8 CAR1 OYE2 orf19.5553 orf19.5597.1 AYR2 HHO1 MIS12 orf19.6415.1 SUI1 HAT2 orf19.6868 orf19.4517 orf19.6435 GSH2 ATP5 orf19.3226 LSC1 orf19.1723 RPS7A POB3 orf19.3690.2 ATP1 RPS15 ATP2 GDH3 RPS25B MES1 PDI1 orf19.1340 PRE6 orf19.716 RPL13 orf19.3061.1;RPS22A;orf19.3061.1 orf19.1394 PDB1 LAT1 RLI1</t>
+          <t>RPS21B orf19.71 ARG5,6 ERG12 RBK1 MUQ1 RPL38 DCK1 BAT21 orf19.6867 orf19.3572.3 ILV2 DTD2 PRE3 HIS5 ERG8 ARG8 CAR1 OYE2 orf19.5553 orf19.5597.1 AYR2 HHO1 MIS12 orf19.6415.1 SUI1 HAT2 orf19.6868 orf19.4517 RPN10 PR26 orf19.6435 GSH2 ATP5 orf19.3226 LSC1 CPR6 orf19.2008 orf19.1723 RPS7A POB3 ADE2 orf19.3690.2 ATP1 RPS15 RPS19A ATP2 GDH3 RPS25B MES1 orf19.6507 PDI1 orf19.1340 PRE6 orf19.716 RPL13 orf19.3061.1;RPS22A;orf19.3061.1 orf19.1394 RPS20 PDB1 CCT8 GRX3 LAT1 RLI1 HOM6</t>
         </is>
       </c>
     </row>
@@ -1992,11 +1997,11 @@
         </is>
       </c>
       <c r="F10">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>GAL7 MMD1 ZWF1 orf19.2296 orf19.7244 orf19.7214 ERG20 orf19.2269 APE3 LEU42 orf19.7437 AAT22 SOD1 COF1 GRE3 orf19.3982 orf19.3482 GCV1 orf19.5773 GBP2 PRE10 CPY1 orf19.7131 orf19.7140 ARC19 PGM2 MLC1 orf19.518 IFE2 ADE13 ARP2 RPO21 ATP16 CAT1 RBP1 ARO4 SOU1 APE2 HEM13 LKH1 orf19.1796 SOL3 CSH1 LYS22 EGD1 orf19.1862 GAL1 CCS1 SKP1 HNT1 PST2 DQD1 SPE3 TFS1 RIB3 GVP36 orf19.5369 MDH1-3 FUM11 MRPL40 orf19.3357 MGE1 GLO1 orf19.2047 SLK19 PRE9 orf19.2737 HSP21 PUT2 CYB2 orf19.4953 orf19.1460 RPP2B BCY1 GAD1 GND1 IDH2 PST1 PRO3 RPP1B CYP1 PGK1 CDC19 MET6 HXK2 UCF1 ICL1 TKL1 SNZ1</t>
+          <t>MMD1 ZWF1 orf19.2296 orf19.7244 orf19.7214 orf19.2269 APE3 orf19.7437 AAT22 SOD1 GRE3 orf19.3982 orf19.3482 GCV1 orf19.5773 GBP2 PRE10 CPY1 orf19.7140 PGM2 MLC1 orf19.518 RPO21 ATP16 ARO4 SOU1 APE2 HEM13 LKH1 CSH1 orf19.1862 GAL1 CCS1 SKP1 HNT1 PST2 DQD1 SPE3 TFS1 orf19.5369 FUM11 MRPL40 MGE1 ARC35 GLO1 orf19.2047 SLK19 PRE9 orf19.2737 HSP21 PUT2 CYB2 orf19.1460 RPP2B GND1 IDH2 PRO3 PGK1 CDC19 MET6 HXK2 TKL1 MET3</t>
         </is>
       </c>
     </row>
@@ -2019,11 +2024,11 @@
         </is>
       </c>
       <c r="F11">
-        <v>142</v>
+        <v>84</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>orf19.3325 orf19.4532 orf19.3684 orf19.3003 orf19.2988 orf19.3016 orf19.1037;IFI3 PRC3 orf19.6211 orf19.5054 UBA2 orf19.4735 NTF2 RPA190 orf19.2305 orf19.670.2 orf19.5239 CDC54 MDG1 orf19.2111 ARO8 RAD23 HYU1 NSP1 orf19.4504 orf19.4492 TPK2 orf19.2214 GLO2 CDC47 orf19.200 MRPL33 PPH21 ALT1 orf19.6966 HAL3 orf19.2686 orf19.5038 ALD6 orf19.1940 orf19.4225.1 orf19.4316 orf19.6658 orf19.3957 RIB5 orf19.92 orf19.3499 STE23 orf19.5730 VPS70 LEU2 ACB1 orf19.5131 HIS7 orf19.7200 orf19.7196 UTP18 POT1 orf19.7499 orf19.6305 orf19.3704.1 TPM2 orf19.7288 PDK2 orf19.6602 orf19.5158 CHS5 DUT1 HIS1 CGR1 ESS1 CTN3 orf19.1857 RPB8 GLY1 CAF16 BUB3 orf19.6693 SPS20 HTA1 CTN1 orf19.5666 GPM2 SMT3 YPD1 orf19.2306 orf19.109 HAL22 GIS2 orf19.2262 MCM2 orf19.5812 ECI1 orf19.5250 MAE1 BDF1 orf19.967 VPS2 orf19.5321 LAP3 orf19.500 CAB3 ISN1 NAA25 orf19.5522 HCR1 YSA1 orf19.6739 orf19.6717 orf19.345 MET13 KEX1 orf19.6585 orf19.6554 orf19.904 GNA1 ACP12 COQ4 FOX3 POX1-3 orf19.3922 DOS2 GCV3 OSM2 TYR1 CLC1 orf19.4894 orf19.4796 PIL1 orf19.6358 FOX2 orf19.3124 orf19.4246 ARD ECM4 UGP1 AAT21 orf19.2335 RPS12 TPS2 ILV3 MLS1</t>
+          <t>orf19.3325 orf19.4532 orf19.3684 orf19.2988 orf19.3016 orf19.1037;IFI3 PRC3 orf19.5054 orf19.4735 NTF2 RPA190 orf19.670.2 MDG1 NSP1 orf19.4504 TPK2 orf19.2214 GLO2 orf19.200 MRPL33 PPH21 ALT1 orf19.5038 ALD6 orf19.4225.1 orf19.4316 orf19.6658 orf19.92 STE23 orf19.5730 ACB1 orf19.7200 POT1 orf19.7499 orf19.3704.1 TPM2 orf19.7288 orf19.6602 orf19.5158 DUT1 HIS1 CTN3 RPB8 BUB3 orf19.6693 GPM2 SMT3 YPD1 orf19.2306 orf19.109 HAL22 orf19.2262 MAE1 BDF1 orf19.967 orf19.5321 LAP3 CAB3 ISN1 NAA25 HCR1 orf19.6739 orf19.345 MET13 KEX1 orf19.6554 orf19.904 ACP12 FOX3 POX1-3 DOS2 GCV3 TYR1 orf19.4894 orf19.4796 PIL1 orf19.2686 ARD LEU2 UGP1 CAF16 MCM2 orf19.6717 TPS2</t>
         </is>
       </c>
     </row>
@@ -2046,11 +2051,11 @@
         </is>
       </c>
       <c r="F12">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>MVD orf19.7269 UGA1 orf19.185 orf19.6160 orf19.1662 HIS4 OFD1 HOM3 RPN8 TIF3 orf19.3480 SBA1 CRN1 orf19.7199 LEU1 ARO2 orf19.6612 orf19.3755 HMO1 orf19.1162 EFG1 ARP3 orf19.2275 orf19.3129 orf19.3442 orf19.969 orf19.498 orf19.5420 orf19.3349 ARC35 orf19.6090 MRT4 SEC13 orf19.4283 orf19.3022 orf19.1687 PDX1 PRS1 URE2 IDP2 SHM2 ANB1 ENO1 SSA2 ACO1 IMH3 FDH1 MIS11 TDH3 HSP78 MET3</t>
+          <t>GAL7 UGA1 orf19.185 orf19.6160 HIS4 OFD1 HOM3 RPN8 TIF3 orf19.3480 SBA1 CRN1 LEU1 ARC19 orf19.6612 orf19.3755 HMO1 orf19.1162 EGD1 EFG1 ARP3 orf19.2275 GVP36 orf19.969 MDH1-3 orf19.498 orf19.5420 orf19.3357 orf19.3349 orf19.6090 MRT4 SEC13 orf19.4283 orf19.3022 orf19.1687 PDX1 orf19.4953 PRS1 URE2 BCY1 RPP1B SHM2 ANB1 ACO1 FDH1 MIS11</t>
         </is>
       </c>
     </row>
@@ -2073,11 +2078,11 @@
         </is>
       </c>
       <c r="F13">
-        <v>191</v>
+        <v>141</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>RPO41 MRP20 LYS2 PDE2 MAS1 orf19.3027 PHO85 orf19.6843 orf19.6853 orf19.6245 ADE4 SMI1 orf19.5095 orf19.989 orf19.2333 RPL82 orf19.2330 NEP1 KEM1 NPL3 orf19.7234 RPC10 orf19.2019 orf19.1444 orf19.1516 ENT3 GCD7 orf19.3559 orf19.3528 orf19.2259 orf19.2278 MCM3 orf19.1389 MET10 orf19.1381 YOR1 RPT2 orf19.1697 UTP4 AIP2 DNM1 orf19.7404 orf19.6718 PTC7 PWP1 MSN5 orf19.2664 RRP42 orf19.1791 ARO9 orf19.1272 orf19.5698 orf19.1953 orf19.1961 orf19.1967 SNF1 MAS2 orf19.6665 orf19.2639.1 GUK1 orf19.4030 orf19.1180 orf19.4193 CIC1 orf19.5747 orf19.73 orf19.1085 orf19.2143 orf19.7097 orf19.7086 RPA135 orf19.7067 YML6 orf19.7012 GCN3 AHP2 orf19.6458.1 orf19.5161 orf19.1335 MRP7 KAP120 orf19.7478 PAN6 orf19.2835 orf19.639.1 CRG1 orf19.7290 ELF1 YKE2 CTM1 MRPS9 CDC21 SPL1 SIT4 CKS1 orf19.4204 orf19.6346 GCF1 orf19.397 orf19.394 orf19.2639 MRPL8 orf19.3477 orf19.213 PPZ1 VMA10 ERB1 orf19.2352 UBA4 PES1 orf19.585 orf19.3585 RFA2 MRPL10 CKA2 orf19.7215 orf19.2920 orf19.439 PRS5 orf19.6424 orf19.5279 orf19.5235 orf19.7291 orf19.1248 orf19.3446 NAM7 orf19.933 orf19.5168 LYS4 MRP8 orf19.3836 orf19.3797 orf19.512 MRPL3 orf19.5393 SKI8 orf19.5757 ZPR1 MET2 ARP9 orf19.2438 MRPL19 PGA63 KEL1 LEU4 ARP4 orf19.6822 SSN6 MET8 orf19.6752 orf19.4306 orf19.6503 orf19.863 COQ6 ARX1 orf19.4021 orf19.4018 orf19.3977 orf19.4932 orf19.1565 orf19.1545 orf19.4611 orf19.4597 MCA1 YTM1 orf19.4751 HBR1 orf19.2930 GLT1 orf19.6220.4 orf19.2095 orf19.2720 CCT6 RPL43A RPL25 RPL23A SUI3 orf19.2520 ARC1 RPS27 GPD1 orf19.2286 ADK1 orf19.5293 RPL15A ADE17 TUF1 ZUO1 orf19.3045 URA7 orf19.5885</t>
+          <t>LYS2 PDE2 MAS1 PHO85 orf19.6853 ADE4 SMI1 orf19.989 orf19.2333 RPL82 orf19.2305 KEM1 NPL3 orf19.7234 RPC10 ARO8 orf19.1444 ENT3 GCD7 orf19.3559 orf19.3528 orf19.2259 orf19.2278 MCM3 orf19.1389 MET10 orf19.1381 YOR1 RPT2 orf19.1697 AIP2 DNM1 orf19.7404 orf19.6718 RRP42 ARO9 orf19.1272 orf19.5698 orf19.1953 orf19.1961 SNF1 orf19.6665 GUK1 RIB5 orf19.1180 orf19.4193 CIC1 orf19.3499 orf19.5747 orf19.73 orf19.1085 orf19.7097 RPA135 orf19.7067 YML6 orf19.7012 GCN3 AHP2 orf19.5161 MRP7 KAP120 orf19.7478 PAN6 orf19.2835 orf19.6305 orf19.639.1 CRG1 orf19.7290 YKE2 CTM1 MRPS9 CDC21 SPL1 SIT4 CKS1 orf19.4204 orf19.6346 GCF1 orf19.394 orf19.2639 MRPL8 orf19.213 CTN1 PPZ1 VMA10 orf19.2352 UBA4 PES1 orf19.585 orf19.3585 GIS2 RFA2 MRPL10 CKA2 orf19.7215 orf19.5812 orf19.2920 orf19.439 PRS5 orf19.6424 orf19.5279 orf19.5235 orf19.1248 orf19.3446 VPS2 orf19.933 LYS4 MRP8 orf19.3797 MRPL3 orf19.5393 ZPR1 MET2 ARP9 orf19.2438 MRPL19 PGA63 LEU4 ARP4 orf19.6822 orf19.6752 orf19.4306 orf19.6503 orf19.863 COQ6 ARX1 COQ4 orf19.4018 orf19.3977 OSM2 orf19.4932 orf19.1565 orf19.4597 CLC1 MCA1 YTM1 orf19.4751 HBR1 RPS27 RPS12 URA7</t>
         </is>
       </c>
     </row>
@@ -2100,11 +2105,11 @@
         </is>
       </c>
       <c r="F14">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>RNR22 ARA1 TPS3 FBP1 orf19.4609 GLC3 PUP3 orf19.7531 ARG1 URA5 RPP2A ASR2 MAL2 TUP1 orf19.3508 ARO10 CYS3 orf19.6065 orf19.6816 GST2 orf19.1709 orf19.3932 AGM1 GDH2 FUM12 GPH1 PCK1 HSP104 orf19.7297 XYL2 HSP70 GLK1;GLK4 PFK2 PFK1 PSA2</t>
+          <t>ERG20 RNR22 ARA1 LEU42 FBP1 HRT2 COF1 EBP1 PUP3 orf19.7199 orf19.7131 orf19.7531 ARG1 URA5 IFE2 ADE13 ARO2 ASR2 ARP2 MAL2 CAT1 TUP1 RBP1 CYC1 orf19.3508 orf19.1796 SOL3 OSM1 LYS22 RIB3 GSY1 orf19.6816 orf19.338 GST2 orf19.1709 orf19.3932 AGM1 GAD1 PST1 GDH2 orf19.2175 FUM12 PYC2 GPH1 PCK1 IDP2 HSP104 orf19.7297 XYL2 CYP1 HSP70 UCF1 ICL1 GLK1;GLK4 CCP1 SNZ1 PFK1 PSA2 HSP78</t>
         </is>
       </c>
     </row>
@@ -2127,11 +2132,11 @@
         </is>
       </c>
       <c r="F15">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>SIN3 IST2 orf19.4888 orf19.4901 orf19.4952.1 orf19.7210 PNG2 orf19.2265 MLP1 UBR1 AGO1 orf19.577 DAP2 RMS1 orf19.7116 orf19.7041 PHM5 MCM6 DOM34 GUT1 MYO5 orf19.6838 orf19.4164 orf19.477 orf19.5763 orf19.2484 MSF1 orf19.6783 GCD2 orf19.320 orf19.2769 RVS161 VPS4 orf19.3947 orf19.1449 orf19.1495 TOA2 SEC7 orf19.4846 PST3 RPN7 ACS1 PRD1 SDS24 RPS26A TPS1 RPL10A</t>
+          <t>SIN3 orf19.3003 orf19.6211 IST2 UBA2 orf19.4888 orf19.4901 orf19.5239 CDC54 orf19.4952.1 orf19.7210 orf19.2111 RAD23 HYU1 orf19.4492 PNG2 orf19.2265 CDC47 orf19.6966 HAL3 MLP1 UBR1 AGO1 orf19.577 orf19.1940 DAP2 RMS1 orf19.3957 orf19.7116 VPS70 orf19.7041 PHM5 orf19.5131 HIS7 orf19.7196 UTP18 MCM6 DOM34 PDK2 CHS5 CGR1 GUT1 ESS1 MYO5 orf19.1857 GLY1 orf19.6838 orf19.4164 SPS20 HTA1 orf19.5666 ECI1 orf19.5250 orf19.500 orf19.477 orf19.5763 orf19.2484 orf19.5522 MSF1 YSA1 orf19.6783 GCD2 orf19.320 orf19.2769 RVS161 VPS4 orf19.6585 GNA1 orf19.3947 orf19.3922 orf19.1449 orf19.1495 TOA2 SEC7 orf19.4846 GLT1 orf19.6358 RIM11;orf19.792 RPT6 FOX2 orf19.4246 ECM4 PST3 RPN7 AAT21 orf19.2335 ACS1 PRD1 PRX1 orf19.5293 SDS24 orf19.891 ILV3 RPS26A RDI1 MLS1 TPS1</t>
         </is>
       </c>
     </row>
@@ -2154,11 +2159,11 @@
         </is>
       </c>
       <c r="F16">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>AGE3 LTP1 DOA1 GCA1;GCA2 orf19.1514 HPT1 orf19.1785 orf19.1626 GTT11 orf19.7357 HRT2 UAP1 EBP1 SEC27 APA2 orf19.6559 ADE1 TRP2 orf19.4395 orf19.7322 CDC11 orf19.2965 PMI1 CDC10 CYC1 orf19.3515 orf19.1815 GLC7 HSM3 OSM1 ARO7 orf19.2304 CCT2 SUP35 orf19.1946 WRS1 NHP2 PFY1 GSY1 HMT1 SVF1 orf19.338 TRR1 orf19.4248 TIF34 orf19.3938 orf19.4633 POL30 orf19.4816 EIF4E FRS2 DAK2 SAM2 ACT1 ERG10 orf19.2175 ASN1 LYS9 CAR2 PYC2 ADH1 GLN1 FDH3 TSA1;TSA1B;TSA1B PMM1 PDC11 YHB1 ADE6 SIS1 TAL1 CCP1 orf19.3915 APT1 RPP1A TPI1 FBA1</t>
+          <t>MVD AGE3 LTP1 DOA1 GCA1;GCA2 orf19.7269 orf19.1514 HPT1 orf19.1785 TPS3 orf19.1662 orf19.1626 GTT11 orf19.7357 orf19.4609 UAP1 SEC27 APA2 GLC3 orf19.6559 ADE1 TRP2 orf19.4395 RPP2A orf19.7322 CDC11 orf19.2965 PMI1 CDC10 orf19.3515 orf19.1815 ARO10 GLC7 HSM3 ARO7 orf19.2304 CCT2 SUP35 orf19.3129 orf19.1946 CYS3 WRS1 orf19.3442 NHP2 PFY1 HMT1 SVF1 orf19.6065 TRR1 orf19.4248 TIF34 orf19.3938 orf19.4633 POL30 orf19.4816 EIF4E FRS2 DAK2 SAM2 ACT1 ERG10 ASN1 LYS9 CAR2 ADH1 GLN1 FDH3 TSA1;TSA1B;TSA1B ENO1 PMM1 SSA2 PDC11 YHB1 ADE6 IMH3 SIS1 TAL1 TDH3 PFK2 orf19.3915 APT1 RPP1A TPI1 FBA1</t>
         </is>
       </c>
     </row>

</xml_diff>